<commit_message>
mod events $ add tabla
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\racing-cayma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0004D61-D27D-49EC-8949-39D7FB82C8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7533459C-FC2F-40D5-BD03-C7F5ED98A083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="430">
   <si>
     <t>XY</t>
   </si>
@@ -1692,7 +1692,7 @@
   <dimension ref="A1:L135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43:L135"/>
+      <selection activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5339,6 +5339,9 @@
       </c>
       <c r="F105" t="s">
         <v>429</v>
+      </c>
+      <c r="G105" t="s">
+        <v>149</v>
       </c>
       <c r="H105" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
quitar output - de los graficos
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\racing-cayma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC80DAA6-1EE5-4C13-8C64-06E54C098C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077BB43E-689D-4722-A5DB-3CBC5CE8D405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1698,7 +1698,7 @@
   <dimension ref="A1:L135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G136" sqref="G136"/>
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4090,7 +4090,7 @@
         <v>230</v>
       </c>
       <c r="F69" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="G69" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
mapa de pases individual
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\racing-cayma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D0B715-6271-4185-BE9F-3AC17BB15E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78422BE4-5F08-43D6-9E01-2EDC73F43DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2353,7 +2353,7 @@
     <t>individual</t>
   </si>
   <si>
-    <t>Fase</t>
+    <t>Event</t>
   </si>
 </sst>
 </file>
@@ -2440,7 +2440,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:N240" totalsRowShown="0">
   <autoFilter ref="A1:N240" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Fase"/>
+    <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Event"/>
     <tableColumn id="2" xr3:uid="{4A939A0F-B787-4665-B94F-35DE80E0B243}" name="start_time"/>
     <tableColumn id="3" xr3:uid="{237002C1-33B1-4A0C-8625-A4F946E3279C}" name="time"/>
     <tableColumn id="4" xr3:uid="{9D5DC911-C5F2-4D28-93C2-CC287EB8C514}" name="end_time"/>
@@ -2749,7 +2749,7 @@
   <dimension ref="A1:N240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
mapa de pases individual2
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\racing-cayma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78422BE4-5F08-43D6-9E01-2EDC73F43DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD36238-4597-4193-B236-124514926DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2317,9 +2317,6 @@
     <t>65;76 57;63</t>
   </si>
   <si>
-    <t>Player</t>
-  </si>
-  <si>
     <t>Desconocido</t>
   </si>
   <si>
@@ -2354,6 +2351,9 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>player</t>
   </si>
 </sst>
 </file>
@@ -2403,7 +2403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2413,6 +2413,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2449,7 +2452,7 @@
     <tableColumn id="9" xr3:uid="{2B9AEE74-8141-415A-8718-C057D71FC210}" name="output"/>
     <tableColumn id="10" xr3:uid="{CA78ED69-994B-4A34-B8BA-562ED05D3D66}" name="Rival"/>
     <tableColumn id="13" xr3:uid="{AA1AD256-EC33-478A-8418-B244C25C1F49}" name="Video"/>
-    <tableColumn id="6" xr3:uid="{684AB30A-FE4C-4A68-9135-AB51377B71D5}" name="Player"/>
+    <tableColumn id="6" xr3:uid="{684AB30A-FE4C-4A68-9135-AB51377B71D5}" name="player"/>
     <tableColumn id="11" xr3:uid="{0D2BFB16-23FC-4D00-90AD-0D752ACC7B98}" name="Nota"/>
     <tableColumn id="12" xr3:uid="{81FA8199-0E5D-43A7-9DB8-350A7DD2B989}" name="Periodo" dataDxfId="0"/>
     <tableColumn id="14" xr3:uid="{1D07032B-D887-446D-81E8-6EF5BC9D9E9B}" name="invertido"/>
@@ -2749,7 +2752,7 @@
   <dimension ref="A1:N240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2765,7 +2768,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -2791,8 +2794,8 @@
       <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
-        <v>765</v>
+      <c r="J1" s="6" t="s">
+        <v>777</v>
       </c>
       <c r="K1" t="s">
         <v>34</v>
@@ -2804,7 +2807,7 @@
         <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -2840,7 +2843,7 @@
         <v>151</v>
       </c>
       <c r="N2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -2879,7 +2882,7 @@
         <v>151</v>
       </c>
       <c r="N3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2918,7 +2921,7 @@
         <v>151</v>
       </c>
       <c r="N4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -2954,7 +2957,7 @@
         <v>151</v>
       </c>
       <c r="N5" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -2993,7 +2996,7 @@
         <v>151</v>
       </c>
       <c r="N6" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -3032,7 +3035,7 @@
         <v>151</v>
       </c>
       <c r="N7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3071,7 +3074,7 @@
         <v>151</v>
       </c>
       <c r="N8" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -3113,7 +3116,7 @@
         <v>151</v>
       </c>
       <c r="N9" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -3152,7 +3155,7 @@
         <v>151</v>
       </c>
       <c r="N10" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -3191,7 +3194,7 @@
         <v>151</v>
       </c>
       <c r="N11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -3230,7 +3233,7 @@
         <v>151</v>
       </c>
       <c r="N12" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -3266,7 +3269,7 @@
         <v>151</v>
       </c>
       <c r="N13" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -3305,7 +3308,7 @@
         <v>151</v>
       </c>
       <c r="N14" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -3344,7 +3347,7 @@
         <v>151</v>
       </c>
       <c r="N15" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -3383,7 +3386,7 @@
         <v>151</v>
       </c>
       <c r="N16" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -3422,7 +3425,7 @@
         <v>151</v>
       </c>
       <c r="N17" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -3461,7 +3464,7 @@
         <v>151</v>
       </c>
       <c r="N18" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -3500,7 +3503,7 @@
         <v>151</v>
       </c>
       <c r="N19" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -3539,7 +3542,7 @@
         <v>151</v>
       </c>
       <c r="N20" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -3578,7 +3581,7 @@
         <v>151</v>
       </c>
       <c r="N21" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -3617,7 +3620,7 @@
         <v>151</v>
       </c>
       <c r="N22" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -3656,7 +3659,7 @@
         <v>151</v>
       </c>
       <c r="N23" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -3692,7 +3695,7 @@
         <v>151</v>
       </c>
       <c r="N24" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -3731,7 +3734,7 @@
         <v>151</v>
       </c>
       <c r="N25" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -3770,7 +3773,7 @@
         <v>151</v>
       </c>
       <c r="N26" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -3809,7 +3812,7 @@
         <v>151</v>
       </c>
       <c r="N27" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3848,7 +3851,7 @@
         <v>151</v>
       </c>
       <c r="N28" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -3887,7 +3890,7 @@
         <v>151</v>
       </c>
       <c r="N29" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -3926,7 +3929,7 @@
         <v>151</v>
       </c>
       <c r="N30" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -3965,7 +3968,7 @@
         <v>151</v>
       </c>
       <c r="N31" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -4001,7 +4004,7 @@
         <v>151</v>
       </c>
       <c r="N32" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -4040,7 +4043,7 @@
         <v>151</v>
       </c>
       <c r="N33" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -4076,7 +4079,7 @@
         <v>151</v>
       </c>
       <c r="N34" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -4115,7 +4118,7 @@
         <v>151</v>
       </c>
       <c r="N35" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -4154,7 +4157,7 @@
         <v>151</v>
       </c>
       <c r="N36" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -4193,7 +4196,7 @@
         <v>151</v>
       </c>
       <c r="N37" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -4232,7 +4235,7 @@
         <v>151</v>
       </c>
       <c r="N38" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -4268,7 +4271,7 @@
         <v>151</v>
       </c>
       <c r="N39" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -4307,7 +4310,7 @@
         <v>151</v>
       </c>
       <c r="N40" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -4346,7 +4349,7 @@
         <v>151</v>
       </c>
       <c r="N41" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -4385,7 +4388,7 @@
         <v>151</v>
       </c>
       <c r="N42" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
@@ -4424,7 +4427,7 @@
         <v>151</v>
       </c>
       <c r="N43" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
@@ -4463,7 +4466,7 @@
         <v>151</v>
       </c>
       <c r="N44" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -4502,7 +4505,7 @@
         <v>151</v>
       </c>
       <c r="N45" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -4541,7 +4544,7 @@
         <v>151</v>
       </c>
       <c r="N46" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -4580,7 +4583,7 @@
         <v>151</v>
       </c>
       <c r="N47" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -4619,7 +4622,7 @@
         <v>151</v>
       </c>
       <c r="N48" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -4658,7 +4661,7 @@
         <v>151</v>
       </c>
       <c r="N49" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -4697,7 +4700,7 @@
         <v>151</v>
       </c>
       <c r="N50" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
@@ -4736,7 +4739,7 @@
         <v>151</v>
       </c>
       <c r="N51" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -4775,7 +4778,7 @@
         <v>151</v>
       </c>
       <c r="N52" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
@@ -4814,7 +4817,7 @@
         <v>151</v>
       </c>
       <c r="N53" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -4853,7 +4856,7 @@
         <v>151</v>
       </c>
       <c r="N54" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
@@ -4892,7 +4895,7 @@
         <v>151</v>
       </c>
       <c r="N55" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -4931,7 +4934,7 @@
         <v>151</v>
       </c>
       <c r="N56" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -4970,7 +4973,7 @@
         <v>151</v>
       </c>
       <c r="N57" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -5009,7 +5012,7 @@
         <v>151</v>
       </c>
       <c r="N58" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -5048,7 +5051,7 @@
         <v>151</v>
       </c>
       <c r="N59" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -5087,7 +5090,7 @@
         <v>151</v>
       </c>
       <c r="N60" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
@@ -5126,7 +5129,7 @@
         <v>151</v>
       </c>
       <c r="N61" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -5165,7 +5168,7 @@
         <v>151</v>
       </c>
       <c r="N62" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -5204,7 +5207,7 @@
         <v>151</v>
       </c>
       <c r="N63" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -5240,7 +5243,7 @@
         <v>151</v>
       </c>
       <c r="N64" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -5279,7 +5282,7 @@
         <v>151</v>
       </c>
       <c r="N65" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -5318,7 +5321,7 @@
         <v>151</v>
       </c>
       <c r="N66" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -5357,7 +5360,7 @@
         <v>151</v>
       </c>
       <c r="N67" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -5396,7 +5399,7 @@
         <v>151</v>
       </c>
       <c r="N68" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -5435,7 +5438,7 @@
         <v>151</v>
       </c>
       <c r="N69" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -5474,7 +5477,7 @@
         <v>151</v>
       </c>
       <c r="N70" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
@@ -5510,7 +5513,7 @@
         <v>151</v>
       </c>
       <c r="N71" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -5549,7 +5552,7 @@
         <v>151</v>
       </c>
       <c r="N72" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -5588,7 +5591,7 @@
         <v>151</v>
       </c>
       <c r="N73" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -5627,7 +5630,7 @@
         <v>151</v>
       </c>
       <c r="N74" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -5666,7 +5669,7 @@
         <v>151</v>
       </c>
       <c r="N75" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -5705,7 +5708,7 @@
         <v>151</v>
       </c>
       <c r="N76" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -5744,7 +5747,7 @@
         <v>151</v>
       </c>
       <c r="N77" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -5783,7 +5786,7 @@
         <v>151</v>
       </c>
       <c r="N78" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -5822,7 +5825,7 @@
         <v>151</v>
       </c>
       <c r="N79" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -5861,7 +5864,7 @@
         <v>151</v>
       </c>
       <c r="N80" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -5900,7 +5903,7 @@
         <v>151</v>
       </c>
       <c r="N81" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -5939,7 +5942,7 @@
         <v>151</v>
       </c>
       <c r="N82" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -5978,7 +5981,7 @@
         <v>151</v>
       </c>
       <c r="N83" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -6017,7 +6020,7 @@
         <v>151</v>
       </c>
       <c r="N84" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -6056,7 +6059,7 @@
         <v>151</v>
       </c>
       <c r="N85" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -6092,7 +6095,7 @@
         <v>151</v>
       </c>
       <c r="N86" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -6131,7 +6134,7 @@
         <v>151</v>
       </c>
       <c r="N87" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -6170,7 +6173,7 @@
         <v>151</v>
       </c>
       <c r="N88" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -6209,7 +6212,7 @@
         <v>151</v>
       </c>
       <c r="N89" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -6248,7 +6251,7 @@
         <v>151</v>
       </c>
       <c r="N90" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -6287,7 +6290,7 @@
         <v>151</v>
       </c>
       <c r="N91" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -6326,7 +6329,7 @@
         <v>151</v>
       </c>
       <c r="N92" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -6365,7 +6368,7 @@
         <v>151</v>
       </c>
       <c r="N93" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -6404,7 +6407,7 @@
         <v>151</v>
       </c>
       <c r="N94" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -6443,7 +6446,7 @@
         <v>151</v>
       </c>
       <c r="N95" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -6482,7 +6485,7 @@
         <v>151</v>
       </c>
       <c r="N96" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -6521,7 +6524,7 @@
         <v>151</v>
       </c>
       <c r="N97" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -6557,7 +6560,7 @@
         <v>151</v>
       </c>
       <c r="N98" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
@@ -6596,7 +6599,7 @@
         <v>151</v>
       </c>
       <c r="N99" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -6638,7 +6641,7 @@
         <v>151</v>
       </c>
       <c r="N100" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
@@ -6677,7 +6680,7 @@
         <v>151</v>
       </c>
       <c r="N101" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -6716,7 +6719,7 @@
         <v>151</v>
       </c>
       <c r="N102" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -6755,7 +6758,7 @@
         <v>151</v>
       </c>
       <c r="N103" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -6794,7 +6797,7 @@
         <v>151</v>
       </c>
       <c r="N104" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -6836,7 +6839,7 @@
         <v>151</v>
       </c>
       <c r="N105" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -6875,7 +6878,7 @@
         <v>151</v>
       </c>
       <c r="N106" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -6914,7 +6917,7 @@
         <v>151</v>
       </c>
       <c r="N107" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -6953,7 +6956,7 @@
         <v>151</v>
       </c>
       <c r="N108" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -6992,7 +6995,7 @@
         <v>151</v>
       </c>
       <c r="N109" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -7031,7 +7034,7 @@
         <v>151</v>
       </c>
       <c r="N110" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -7070,7 +7073,7 @@
         <v>151</v>
       </c>
       <c r="N111" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
@@ -7109,7 +7112,7 @@
         <v>151</v>
       </c>
       <c r="N112" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -7148,7 +7151,7 @@
         <v>151</v>
       </c>
       <c r="N113" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
@@ -7187,7 +7190,7 @@
         <v>151</v>
       </c>
       <c r="N114" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
@@ -7226,7 +7229,7 @@
         <v>151</v>
       </c>
       <c r="N115" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
@@ -7265,7 +7268,7 @@
         <v>151</v>
       </c>
       <c r="N116" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
@@ -7304,7 +7307,7 @@
         <v>151</v>
       </c>
       <c r="N117" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
@@ -7340,7 +7343,7 @@
         <v>151</v>
       </c>
       <c r="N118" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
@@ -7379,7 +7382,7 @@
         <v>151</v>
       </c>
       <c r="N119" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
@@ -7418,7 +7421,7 @@
         <v>151</v>
       </c>
       <c r="N120" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
@@ -7457,7 +7460,7 @@
         <v>151</v>
       </c>
       <c r="N121" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
@@ -7496,7 +7499,7 @@
         <v>151</v>
       </c>
       <c r="N122" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
@@ -7535,7 +7538,7 @@
         <v>151</v>
       </c>
       <c r="N123" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
@@ -7574,7 +7577,7 @@
         <v>151</v>
       </c>
       <c r="N124" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
@@ -7613,7 +7616,7 @@
         <v>151</v>
       </c>
       <c r="N125" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
@@ -7652,7 +7655,7 @@
         <v>151</v>
       </c>
       <c r="N126" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
@@ -7691,7 +7694,7 @@
         <v>151</v>
       </c>
       <c r="N127" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
@@ -7730,7 +7733,7 @@
         <v>151</v>
       </c>
       <c r="N128" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
@@ -7769,7 +7772,7 @@
         <v>151</v>
       </c>
       <c r="N129" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
@@ -7808,7 +7811,7 @@
         <v>151</v>
       </c>
       <c r="N130" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
@@ -7847,7 +7850,7 @@
         <v>151</v>
       </c>
       <c r="N131" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
@@ -7886,7 +7889,7 @@
         <v>151</v>
       </c>
       <c r="N132" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
@@ -7925,7 +7928,7 @@
         <v>151</v>
       </c>
       <c r="N133" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
@@ -7964,7 +7967,7 @@
         <v>151</v>
       </c>
       <c r="N134" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
@@ -8003,7 +8006,7 @@
         <v>151</v>
       </c>
       <c r="N135" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
@@ -8023,7 +8026,7 @@
         <v>432</v>
       </c>
       <c r="G136" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H136" t="s">
         <v>149</v>
@@ -8032,7 +8035,7 @@
         <v>150</v>
       </c>
       <c r="J136" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L136" s="2" t="s">
         <v>8</v>
@@ -8041,7 +8044,7 @@
         <v>151</v>
       </c>
       <c r="N136" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
@@ -8061,7 +8064,7 @@
         <v>435</v>
       </c>
       <c r="G137" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H137" t="s">
         <v>149</v>
@@ -8070,7 +8073,7 @@
         <v>150</v>
       </c>
       <c r="J137" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L137" s="2" t="s">
         <v>8</v>
@@ -8079,7 +8082,7 @@
         <v>151</v>
       </c>
       <c r="N137" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
@@ -8099,7 +8102,7 @@
         <v>439</v>
       </c>
       <c r="G138" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H138" t="s">
         <v>149</v>
@@ -8108,7 +8111,7 @@
         <v>150</v>
       </c>
       <c r="J138" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L138" s="2" t="s">
         <v>8</v>
@@ -8117,7 +8120,7 @@
         <v>151</v>
       </c>
       <c r="N138" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
@@ -8137,7 +8140,7 @@
         <v>440</v>
       </c>
       <c r="G139" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H139" t="s">
         <v>149</v>
@@ -8146,7 +8149,7 @@
         <v>150</v>
       </c>
       <c r="J139" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L139" s="2" t="s">
         <v>8</v>
@@ -8155,7 +8158,7 @@
         <v>151</v>
       </c>
       <c r="N139" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
@@ -8175,7 +8178,7 @@
         <v>444</v>
       </c>
       <c r="G140" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H140" t="s">
         <v>149</v>
@@ -8184,7 +8187,7 @@
         <v>150</v>
       </c>
       <c r="J140" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>8</v>
@@ -8193,7 +8196,7 @@
         <v>151</v>
       </c>
       <c r="N140" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
@@ -8213,7 +8216,7 @@
         <v>447</v>
       </c>
       <c r="G141" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H141" t="s">
         <v>149</v>
@@ -8222,7 +8225,7 @@
         <v>150</v>
       </c>
       <c r="J141" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L141" s="2" t="s">
         <v>8</v>
@@ -8231,7 +8234,7 @@
         <v>151</v>
       </c>
       <c r="N141" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
@@ -8251,7 +8254,7 @@
         <v>449</v>
       </c>
       <c r="G142" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H142" t="s">
         <v>149</v>
@@ -8260,7 +8263,7 @@
         <v>150</v>
       </c>
       <c r="J142" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L142" s="2" t="s">
         <v>8</v>
@@ -8269,7 +8272,7 @@
         <v>151</v>
       </c>
       <c r="N142" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
@@ -8289,7 +8292,7 @@
         <v>453</v>
       </c>
       <c r="G143" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H143" t="s">
         <v>149</v>
@@ -8298,7 +8301,7 @@
         <v>150</v>
       </c>
       <c r="J143" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L143" s="2" t="s">
         <v>8</v>
@@ -8307,7 +8310,7 @@
         <v>151</v>
       </c>
       <c r="N143" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
@@ -8327,7 +8330,7 @@
         <v>456</v>
       </c>
       <c r="G144" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H144" t="s">
         <v>149</v>
@@ -8336,7 +8339,7 @@
         <v>150</v>
       </c>
       <c r="J144" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L144" s="2" t="s">
         <v>8</v>
@@ -8345,7 +8348,7 @@
         <v>151</v>
       </c>
       <c r="N144" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
@@ -8365,7 +8368,7 @@
         <v>459</v>
       </c>
       <c r="G145" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H145" t="s">
         <v>149</v>
@@ -8374,7 +8377,7 @@
         <v>150</v>
       </c>
       <c r="J145" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L145" s="2" t="s">
         <v>8</v>
@@ -8383,7 +8386,7 @@
         <v>151</v>
       </c>
       <c r="N145" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
@@ -8403,7 +8406,7 @@
         <v>463</v>
       </c>
       <c r="G146" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H146" t="s">
         <v>149</v>
@@ -8412,7 +8415,7 @@
         <v>150</v>
       </c>
       <c r="J146" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L146" s="2" t="s">
         <v>8</v>
@@ -8421,7 +8424,7 @@
         <v>151</v>
       </c>
       <c r="N146" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
@@ -8441,7 +8444,7 @@
         <v>466</v>
       </c>
       <c r="G147" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H147" t="s">
         <v>149</v>
@@ -8450,7 +8453,7 @@
         <v>150</v>
       </c>
       <c r="J147" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L147" s="2" t="s">
         <v>8</v>
@@ -8459,7 +8462,7 @@
         <v>151</v>
       </c>
       <c r="N147" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
@@ -8479,7 +8482,7 @@
         <v>470</v>
       </c>
       <c r="G148" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H148" t="s">
         <v>149</v>
@@ -8488,7 +8491,7 @@
         <v>150</v>
       </c>
       <c r="J148" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L148" s="2" t="s">
         <v>8</v>
@@ -8497,7 +8500,7 @@
         <v>151</v>
       </c>
       <c r="N148" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
@@ -8517,7 +8520,7 @@
         <v>474</v>
       </c>
       <c r="G149" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H149" t="s">
         <v>149</v>
@@ -8526,7 +8529,7 @@
         <v>150</v>
       </c>
       <c r="J149" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L149" s="2" t="s">
         <v>8</v>
@@ -8535,7 +8538,7 @@
         <v>151</v>
       </c>
       <c r="N149" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
@@ -8555,7 +8558,7 @@
         <v>476</v>
       </c>
       <c r="G150" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H150" t="s">
         <v>149</v>
@@ -8564,7 +8567,7 @@
         <v>150</v>
       </c>
       <c r="J150" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L150" s="2" t="s">
         <v>8</v>
@@ -8573,7 +8576,7 @@
         <v>151</v>
       </c>
       <c r="N150" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
@@ -8593,7 +8596,7 @@
         <v>479</v>
       </c>
       <c r="G151" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H151" t="s">
         <v>149</v>
@@ -8602,7 +8605,7 @@
         <v>150</v>
       </c>
       <c r="J151" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L151" s="2" t="s">
         <v>8</v>
@@ -8611,7 +8614,7 @@
         <v>151</v>
       </c>
       <c r="N151" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
@@ -8631,7 +8634,7 @@
         <v>482</v>
       </c>
       <c r="G152" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H152" t="s">
         <v>149</v>
@@ -8640,7 +8643,7 @@
         <v>150</v>
       </c>
       <c r="J152" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L152" s="2" t="s">
         <v>8</v>
@@ -8649,7 +8652,7 @@
         <v>151</v>
       </c>
       <c r="N152" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
@@ -8669,7 +8672,7 @@
         <v>486</v>
       </c>
       <c r="G153" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H153" t="s">
         <v>149</v>
@@ -8678,7 +8681,7 @@
         <v>150</v>
       </c>
       <c r="J153" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L153" s="2" t="s">
         <v>8</v>
@@ -8687,7 +8690,7 @@
         <v>151</v>
       </c>
       <c r="N153" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
@@ -8707,7 +8710,7 @@
         <v>488</v>
       </c>
       <c r="G154" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H154" t="s">
         <v>149</v>
@@ -8716,7 +8719,7 @@
         <v>150</v>
       </c>
       <c r="J154" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L154" s="2" t="s">
         <v>8</v>
@@ -8725,7 +8728,7 @@
         <v>151</v>
       </c>
       <c r="N154" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
@@ -8745,7 +8748,7 @@
         <v>489</v>
       </c>
       <c r="G155" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H155" t="s">
         <v>149</v>
@@ -8754,7 +8757,7 @@
         <v>150</v>
       </c>
       <c r="J155" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L155" s="2" t="s">
         <v>8</v>
@@ -8763,7 +8766,7 @@
         <v>151</v>
       </c>
       <c r="N155" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
@@ -8783,7 +8786,7 @@
         <v>492</v>
       </c>
       <c r="G156" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H156" t="s">
         <v>149</v>
@@ -8792,7 +8795,7 @@
         <v>150</v>
       </c>
       <c r="J156" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L156" s="2" t="s">
         <v>8</v>
@@ -8801,7 +8804,7 @@
         <v>151</v>
       </c>
       <c r="N156" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
@@ -8821,7 +8824,7 @@
         <v>496</v>
       </c>
       <c r="G157" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H157" t="s">
         <v>149</v>
@@ -8830,7 +8833,7 @@
         <v>150</v>
       </c>
       <c r="J157" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L157" s="2" t="s">
         <v>8</v>
@@ -8839,7 +8842,7 @@
         <v>151</v>
       </c>
       <c r="N157" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
@@ -8859,7 +8862,7 @@
         <v>499</v>
       </c>
       <c r="G158" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H158" t="s">
         <v>149</v>
@@ -8868,7 +8871,7 @@
         <v>150</v>
       </c>
       <c r="J158" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L158" s="2" t="s">
         <v>8</v>
@@ -8877,7 +8880,7 @@
         <v>151</v>
       </c>
       <c r="N158" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
@@ -8897,7 +8900,7 @@
         <v>502</v>
       </c>
       <c r="G159" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H159" t="s">
         <v>149</v>
@@ -8906,7 +8909,7 @@
         <v>150</v>
       </c>
       <c r="J159" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L159" s="2" t="s">
         <v>8</v>
@@ -8915,7 +8918,7 @@
         <v>151</v>
       </c>
       <c r="N159" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
@@ -8935,7 +8938,7 @@
         <v>506</v>
       </c>
       <c r="G160" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H160" t="s">
         <v>149</v>
@@ -8944,7 +8947,7 @@
         <v>150</v>
       </c>
       <c r="J160" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L160" s="2" t="s">
         <v>8</v>
@@ -8953,7 +8956,7 @@
         <v>151</v>
       </c>
       <c r="N160" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.2">
@@ -8973,7 +8976,7 @@
         <v>509</v>
       </c>
       <c r="G161" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H161" t="s">
         <v>149</v>
@@ -8982,7 +8985,7 @@
         <v>150</v>
       </c>
       <c r="J161" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L161" s="2" t="s">
         <v>8</v>
@@ -8991,7 +8994,7 @@
         <v>151</v>
       </c>
       <c r="N161" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
@@ -9011,7 +9014,7 @@
         <v>512</v>
       </c>
       <c r="G162" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H162" t="s">
         <v>149</v>
@@ -9020,7 +9023,7 @@
         <v>150</v>
       </c>
       <c r="J162" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L162" s="2" t="s">
         <v>8</v>
@@ -9029,7 +9032,7 @@
         <v>151</v>
       </c>
       <c r="N162" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.2">
@@ -9049,7 +9052,7 @@
         <v>515</v>
       </c>
       <c r="G163" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H163" t="s">
         <v>149</v>
@@ -9058,7 +9061,7 @@
         <v>150</v>
       </c>
       <c r="J163" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L163" s="2" t="s">
         <v>8</v>
@@ -9067,7 +9070,7 @@
         <v>151</v>
       </c>
       <c r="N163" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
@@ -9087,7 +9090,7 @@
         <v>518</v>
       </c>
       <c r="G164" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H164" t="s">
         <v>149</v>
@@ -9096,7 +9099,7 @@
         <v>150</v>
       </c>
       <c r="J164" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L164" s="2" t="s">
         <v>8</v>
@@ -9105,7 +9108,7 @@
         <v>151</v>
       </c>
       <c r="N164" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.2">
@@ -9125,7 +9128,7 @@
         <v>521</v>
       </c>
       <c r="G165" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H165" t="s">
         <v>149</v>
@@ -9134,7 +9137,7 @@
         <v>150</v>
       </c>
       <c r="J165" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L165" s="2" t="s">
         <v>8</v>
@@ -9143,7 +9146,7 @@
         <v>151</v>
       </c>
       <c r="N165" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.2">
@@ -9163,7 +9166,7 @@
         <v>524</v>
       </c>
       <c r="G166" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H166" t="s">
         <v>149</v>
@@ -9172,7 +9175,7 @@
         <v>150</v>
       </c>
       <c r="J166" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L166" s="2" t="s">
         <v>8</v>
@@ -9181,7 +9184,7 @@
         <v>151</v>
       </c>
       <c r="N166" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.2">
@@ -9201,7 +9204,7 @@
         <v>527</v>
       </c>
       <c r="G167" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H167" t="s">
         <v>149</v>
@@ -9210,7 +9213,7 @@
         <v>150</v>
       </c>
       <c r="J167" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L167" s="2" t="s">
         <v>8</v>
@@ -9219,7 +9222,7 @@
         <v>151</v>
       </c>
       <c r="N167" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.2">
@@ -9239,7 +9242,7 @@
         <v>530</v>
       </c>
       <c r="G168" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H168" t="s">
         <v>149</v>
@@ -9248,7 +9251,7 @@
         <v>150</v>
       </c>
       <c r="J168" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L168" s="2" t="s">
         <v>8</v>
@@ -9257,7 +9260,7 @@
         <v>151</v>
       </c>
       <c r="N168" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.2">
@@ -9277,7 +9280,7 @@
         <v>533</v>
       </c>
       <c r="G169" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H169" t="s">
         <v>149</v>
@@ -9286,7 +9289,7 @@
         <v>150</v>
       </c>
       <c r="J169" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L169" s="2" t="s">
         <v>8</v>
@@ -9295,7 +9298,7 @@
         <v>151</v>
       </c>
       <c r="N169" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.2">
@@ -9315,7 +9318,7 @@
         <v>536</v>
       </c>
       <c r="G170" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H170" t="s">
         <v>149</v>
@@ -9324,7 +9327,7 @@
         <v>150</v>
       </c>
       <c r="J170" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L170" s="2" t="s">
         <v>8</v>
@@ -9333,7 +9336,7 @@
         <v>151</v>
       </c>
       <c r="N170" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.2">
@@ -9353,7 +9356,7 @@
         <v>539</v>
       </c>
       <c r="G171" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H171" t="s">
         <v>149</v>
@@ -9362,7 +9365,7 @@
         <v>150</v>
       </c>
       <c r="J171" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L171" s="2" t="s">
         <v>8</v>
@@ -9371,7 +9374,7 @@
         <v>151</v>
       </c>
       <c r="N171" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.2">
@@ -9391,7 +9394,7 @@
         <v>543</v>
       </c>
       <c r="G172" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H172" t="s">
         <v>149</v>
@@ -9400,7 +9403,7 @@
         <v>150</v>
       </c>
       <c r="J172" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L172" s="2" t="s">
         <v>8</v>
@@ -9409,7 +9412,7 @@
         <v>151</v>
       </c>
       <c r="N172" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.2">
@@ -9429,7 +9432,7 @@
         <v>547</v>
       </c>
       <c r="G173" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H173" t="s">
         <v>149</v>
@@ -9438,7 +9441,7 @@
         <v>150</v>
       </c>
       <c r="J173" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L173" s="2" t="s">
         <v>8</v>
@@ -9447,7 +9450,7 @@
         <v>151</v>
       </c>
       <c r="N173" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.2">
@@ -9467,7 +9470,7 @@
         <v>549</v>
       </c>
       <c r="G174" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H174" t="s">
         <v>149</v>
@@ -9476,7 +9479,7 @@
         <v>150</v>
       </c>
       <c r="J174" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L174" s="2" t="s">
         <v>8</v>
@@ -9485,7 +9488,7 @@
         <v>151</v>
       </c>
       <c r="N174" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.2">
@@ -9505,7 +9508,7 @@
         <v>553</v>
       </c>
       <c r="G175" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H175" t="s">
         <v>149</v>
@@ -9514,7 +9517,7 @@
         <v>150</v>
       </c>
       <c r="J175" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L175" s="2" t="s">
         <v>8</v>
@@ -9523,7 +9526,7 @@
         <v>151</v>
       </c>
       <c r="N175" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.2">
@@ -9543,7 +9546,7 @@
         <v>557</v>
       </c>
       <c r="G176" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H176" t="s">
         <v>149</v>
@@ -9552,7 +9555,7 @@
         <v>150</v>
       </c>
       <c r="J176" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L176" s="2" t="s">
         <v>8</v>
@@ -9561,7 +9564,7 @@
         <v>151</v>
       </c>
       <c r="N176" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.2">
@@ -9581,7 +9584,7 @@
         <v>560</v>
       </c>
       <c r="G177" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H177" t="s">
         <v>149</v>
@@ -9590,7 +9593,7 @@
         <v>150</v>
       </c>
       <c r="J177" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L177" s="2" t="s">
         <v>8</v>
@@ -9599,7 +9602,7 @@
         <v>151</v>
       </c>
       <c r="N177" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.2">
@@ -9619,7 +9622,7 @@
         <v>563</v>
       </c>
       <c r="G178" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H178" t="s">
         <v>149</v>
@@ -9628,7 +9631,7 @@
         <v>150</v>
       </c>
       <c r="J178" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L178" s="2" t="s">
         <v>8</v>
@@ -9637,7 +9640,7 @@
         <v>151</v>
       </c>
       <c r="N178" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.2">
@@ -9657,7 +9660,7 @@
         <v>565</v>
       </c>
       <c r="G179" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H179" t="s">
         <v>149</v>
@@ -9666,7 +9669,7 @@
         <v>150</v>
       </c>
       <c r="J179" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L179" s="2" t="s">
         <v>8</v>
@@ -9675,7 +9678,7 @@
         <v>151</v>
       </c>
       <c r="N179" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.2">
@@ -9695,7 +9698,7 @@
         <v>567</v>
       </c>
       <c r="G180" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H180" t="s">
         <v>149</v>
@@ -9704,7 +9707,7 @@
         <v>150</v>
       </c>
       <c r="J180" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L180" s="2" t="s">
         <v>8</v>
@@ -9713,7 +9716,7 @@
         <v>151</v>
       </c>
       <c r="N180" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.2">
@@ -9733,7 +9736,7 @@
         <v>570</v>
       </c>
       <c r="G181" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H181" t="s">
         <v>149</v>
@@ -9742,7 +9745,7 @@
         <v>150</v>
       </c>
       <c r="J181" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L181" s="2" t="s">
         <v>8</v>
@@ -9751,7 +9754,7 @@
         <v>151</v>
       </c>
       <c r="N181" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.2">
@@ -9771,7 +9774,7 @@
         <v>573</v>
       </c>
       <c r="G182" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H182" t="s">
         <v>149</v>
@@ -9780,7 +9783,7 @@
         <v>150</v>
       </c>
       <c r="J182" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L182" s="2" t="s">
         <v>8</v>
@@ -9789,7 +9792,7 @@
         <v>151</v>
       </c>
       <c r="N182" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.2">
@@ -9809,7 +9812,7 @@
         <v>576</v>
       </c>
       <c r="G183" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H183" t="s">
         <v>149</v>
@@ -9818,7 +9821,7 @@
         <v>150</v>
       </c>
       <c r="J183" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L183" s="2" t="s">
         <v>8</v>
@@ -9827,7 +9830,7 @@
         <v>151</v>
       </c>
       <c r="N183" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.2">
@@ -9847,7 +9850,7 @@
         <v>580</v>
       </c>
       <c r="G184" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H184" t="s">
         <v>149</v>
@@ -9856,7 +9859,7 @@
         <v>150</v>
       </c>
       <c r="J184" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L184" s="2" t="s">
         <v>8</v>
@@ -9865,7 +9868,7 @@
         <v>151</v>
       </c>
       <c r="N184" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.2">
@@ -9885,7 +9888,7 @@
         <v>583</v>
       </c>
       <c r="G185" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H185" t="s">
         <v>149</v>
@@ -9894,7 +9897,7 @@
         <v>150</v>
       </c>
       <c r="J185" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L185" s="2" t="s">
         <v>8</v>
@@ -9903,7 +9906,7 @@
         <v>151</v>
       </c>
       <c r="N185" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.2">
@@ -9923,7 +9926,7 @@
         <v>585</v>
       </c>
       <c r="G186" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H186" t="s">
         <v>149</v>
@@ -9932,7 +9935,7 @@
         <v>150</v>
       </c>
       <c r="J186" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L186" s="2" t="s">
         <v>8</v>
@@ -9941,7 +9944,7 @@
         <v>151</v>
       </c>
       <c r="N186" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.2">
@@ -9961,7 +9964,7 @@
         <v>588</v>
       </c>
       <c r="G187" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H187" t="s">
         <v>149</v>
@@ -9970,7 +9973,7 @@
         <v>150</v>
       </c>
       <c r="J187" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L187" s="2" t="s">
         <v>8</v>
@@ -9979,7 +9982,7 @@
         <v>151</v>
       </c>
       <c r="N187" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.2">
@@ -9999,7 +10002,7 @@
         <v>591</v>
       </c>
       <c r="G188" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H188" t="s">
         <v>149</v>
@@ -10008,7 +10011,7 @@
         <v>150</v>
       </c>
       <c r="J188" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L188" s="2" t="s">
         <v>8</v>
@@ -10017,7 +10020,7 @@
         <v>151</v>
       </c>
       <c r="N188" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.2">
@@ -10037,7 +10040,7 @@
         <v>593</v>
       </c>
       <c r="G189" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H189" t="s">
         <v>149</v>
@@ -10046,7 +10049,7 @@
         <v>150</v>
       </c>
       <c r="J189" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L189" s="2" t="s">
         <v>8</v>
@@ -10055,7 +10058,7 @@
         <v>151</v>
       </c>
       <c r="N189" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="190" spans="1:14" x14ac:dyDescent="0.2">
@@ -10075,7 +10078,7 @@
         <v>596</v>
       </c>
       <c r="G190" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H190" t="s">
         <v>149</v>
@@ -10084,7 +10087,7 @@
         <v>150</v>
       </c>
       <c r="J190" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L190" s="2" t="s">
         <v>8</v>
@@ -10093,7 +10096,7 @@
         <v>151</v>
       </c>
       <c r="N190" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="191" spans="1:14" x14ac:dyDescent="0.2">
@@ -10113,7 +10116,7 @@
         <v>599</v>
       </c>
       <c r="G191" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H191" t="s">
         <v>149</v>
@@ -10122,7 +10125,7 @@
         <v>150</v>
       </c>
       <c r="J191" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L191" s="2" t="s">
         <v>8</v>
@@ -10131,7 +10134,7 @@
         <v>151</v>
       </c>
       <c r="N191" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.2">
@@ -10151,7 +10154,7 @@
         <v>602</v>
       </c>
       <c r="G192" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H192" t="s">
         <v>149</v>
@@ -10160,7 +10163,7 @@
         <v>150</v>
       </c>
       <c r="J192" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L192" s="2" t="s">
         <v>8</v>
@@ -10169,7 +10172,7 @@
         <v>151</v>
       </c>
       <c r="N192" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.2">
@@ -10189,7 +10192,7 @@
         <v>605</v>
       </c>
       <c r="G193" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H193" t="s">
         <v>149</v>
@@ -10198,7 +10201,7 @@
         <v>150</v>
       </c>
       <c r="J193" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L193" s="2" t="s">
         <v>8</v>
@@ -10207,7 +10210,7 @@
         <v>151</v>
       </c>
       <c r="N193" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.2">
@@ -10227,7 +10230,7 @@
         <v>609</v>
       </c>
       <c r="G194" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H194" t="s">
         <v>149</v>
@@ -10236,7 +10239,7 @@
         <v>150</v>
       </c>
       <c r="J194" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L194" s="2" t="s">
         <v>8</v>
@@ -10245,7 +10248,7 @@
         <v>151</v>
       </c>
       <c r="N194" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.2">
@@ -10265,7 +10268,7 @@
         <v>613</v>
       </c>
       <c r="G195" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H195" t="s">
         <v>149</v>
@@ -10274,7 +10277,7 @@
         <v>150</v>
       </c>
       <c r="J195" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L195" s="2" t="s">
         <v>8</v>
@@ -10283,7 +10286,7 @@
         <v>151</v>
       </c>
       <c r="N195" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.2">
@@ -10303,7 +10306,7 @@
         <v>616</v>
       </c>
       <c r="G196" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H196" t="s">
         <v>149</v>
@@ -10312,7 +10315,7 @@
         <v>150</v>
       </c>
       <c r="J196" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L196" s="2" t="s">
         <v>8</v>
@@ -10321,7 +10324,7 @@
         <v>151</v>
       </c>
       <c r="N196" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.2">
@@ -10341,7 +10344,7 @@
         <v>619</v>
       </c>
       <c r="G197" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H197" t="s">
         <v>149</v>
@@ -10350,7 +10353,7 @@
         <v>150</v>
       </c>
       <c r="J197" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L197" s="2" t="s">
         <v>8</v>
@@ -10359,7 +10362,7 @@
         <v>151</v>
       </c>
       <c r="N197" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.2">
@@ -10379,7 +10382,7 @@
         <v>623</v>
       </c>
       <c r="G198" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H198" t="s">
         <v>149</v>
@@ -10388,7 +10391,7 @@
         <v>150</v>
       </c>
       <c r="J198" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L198" s="2" t="s">
         <v>8</v>
@@ -10397,7 +10400,7 @@
         <v>151</v>
       </c>
       <c r="N198" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.2">
@@ -10417,7 +10420,7 @@
         <v>625</v>
       </c>
       <c r="G199" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H199" t="s">
         <v>149</v>
@@ -10426,7 +10429,7 @@
         <v>150</v>
       </c>
       <c r="J199" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L199" s="2" t="s">
         <v>8</v>
@@ -10435,7 +10438,7 @@
         <v>151</v>
       </c>
       <c r="N199" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.2">
@@ -10455,7 +10458,7 @@
         <v>629</v>
       </c>
       <c r="G200" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H200" t="s">
         <v>149</v>
@@ -10464,7 +10467,7 @@
         <v>150</v>
       </c>
       <c r="J200" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L200" s="2" t="s">
         <v>8</v>
@@ -10473,7 +10476,7 @@
         <v>151</v>
       </c>
       <c r="N200" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.2">
@@ -10493,7 +10496,7 @@
         <v>633</v>
       </c>
       <c r="G201" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H201" t="s">
         <v>149</v>
@@ -10502,7 +10505,7 @@
         <v>150</v>
       </c>
       <c r="J201" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L201" s="2" t="s">
         <v>8</v>
@@ -10511,7 +10514,7 @@
         <v>151</v>
       </c>
       <c r="N201" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.2">
@@ -10531,7 +10534,7 @@
         <v>637</v>
       </c>
       <c r="G202" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H202" t="s">
         <v>149</v>
@@ -10540,7 +10543,7 @@
         <v>150</v>
       </c>
       <c r="J202" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L202" s="2" t="s">
         <v>8</v>
@@ -10549,7 +10552,7 @@
         <v>151</v>
       </c>
       <c r="N202" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.2">
@@ -10569,7 +10572,7 @@
         <v>640</v>
       </c>
       <c r="G203" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H203" t="s">
         <v>149</v>
@@ -10578,7 +10581,7 @@
         <v>150</v>
       </c>
       <c r="J203" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L203" s="2" t="s">
         <v>8</v>
@@ -10587,7 +10590,7 @@
         <v>151</v>
       </c>
       <c r="N203" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.2">
@@ -10607,7 +10610,7 @@
         <v>643</v>
       </c>
       <c r="G204" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H204" t="s">
         <v>149</v>
@@ -10616,7 +10619,7 @@
         <v>150</v>
       </c>
       <c r="J204" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L204" s="2" t="s">
         <v>8</v>
@@ -10625,7 +10628,7 @@
         <v>151</v>
       </c>
       <c r="N204" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.2">
@@ -10645,7 +10648,7 @@
         <v>646</v>
       </c>
       <c r="G205" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H205" t="s">
         <v>149</v>
@@ -10654,7 +10657,7 @@
         <v>150</v>
       </c>
       <c r="J205" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L205" s="2" t="s">
         <v>8</v>
@@ -10663,7 +10666,7 @@
         <v>151</v>
       </c>
       <c r="N205" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.2">
@@ -10683,7 +10686,7 @@
         <v>650</v>
       </c>
       <c r="G206" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H206" t="s">
         <v>149</v>
@@ -10692,7 +10695,7 @@
         <v>150</v>
       </c>
       <c r="J206" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L206" s="2" t="s">
         <v>8</v>
@@ -10701,7 +10704,7 @@
         <v>151</v>
       </c>
       <c r="N206" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="207" spans="1:14" x14ac:dyDescent="0.2">
@@ -10721,7 +10724,7 @@
         <v>653</v>
       </c>
       <c r="G207" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H207" t="s">
         <v>149</v>
@@ -10730,7 +10733,7 @@
         <v>150</v>
       </c>
       <c r="J207" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L207" s="2" t="s">
         <v>8</v>
@@ -10739,7 +10742,7 @@
         <v>151</v>
       </c>
       <c r="N207" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.2">
@@ -10759,7 +10762,7 @@
         <v>657</v>
       </c>
       <c r="G208" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H208" t="s">
         <v>149</v>
@@ -10768,7 +10771,7 @@
         <v>150</v>
       </c>
       <c r="J208" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L208" s="2" t="s">
         <v>8</v>
@@ -10777,7 +10780,7 @@
         <v>151</v>
       </c>
       <c r="N208" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.2">
@@ -10797,7 +10800,7 @@
         <v>659</v>
       </c>
       <c r="G209" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H209" t="s">
         <v>149</v>
@@ -10806,7 +10809,7 @@
         <v>150</v>
       </c>
       <c r="J209" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L209" s="2" t="s">
         <v>8</v>
@@ -10815,7 +10818,7 @@
         <v>151</v>
       </c>
       <c r="N209" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.2">
@@ -10835,7 +10838,7 @@
         <v>663</v>
       </c>
       <c r="G210" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H210" t="s">
         <v>149</v>
@@ -10844,7 +10847,7 @@
         <v>150</v>
       </c>
       <c r="J210" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L210" s="2" t="s">
         <v>8</v>
@@ -10853,7 +10856,7 @@
         <v>151</v>
       </c>
       <c r="N210" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.2">
@@ -10873,7 +10876,7 @@
         <v>666</v>
       </c>
       <c r="G211" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H211" t="s">
         <v>149</v>
@@ -10882,7 +10885,7 @@
         <v>150</v>
       </c>
       <c r="J211" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L211" s="2" t="s">
         <v>8</v>
@@ -10891,7 +10894,7 @@
         <v>151</v>
       </c>
       <c r="N211" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.2">
@@ -10911,7 +10914,7 @@
         <v>669</v>
       </c>
       <c r="G212" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H212" t="s">
         <v>149</v>
@@ -10920,7 +10923,7 @@
         <v>150</v>
       </c>
       <c r="J212" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L212" s="2" t="s">
         <v>8</v>
@@ -10929,7 +10932,7 @@
         <v>151</v>
       </c>
       <c r="N212" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.2">
@@ -10949,7 +10952,7 @@
         <v>673</v>
       </c>
       <c r="G213" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H213" t="s">
         <v>149</v>
@@ -10958,7 +10961,7 @@
         <v>150</v>
       </c>
       <c r="J213" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L213" s="2" t="s">
         <v>8</v>
@@ -10967,7 +10970,7 @@
         <v>151</v>
       </c>
       <c r="N213" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.2">
@@ -10987,7 +10990,7 @@
         <v>676</v>
       </c>
       <c r="G214" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H214" t="s">
         <v>149</v>
@@ -10996,7 +10999,7 @@
         <v>150</v>
       </c>
       <c r="J214" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L214" s="2" t="s">
         <v>8</v>
@@ -11005,7 +11008,7 @@
         <v>151</v>
       </c>
       <c r="N214" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="215" spans="1:14" x14ac:dyDescent="0.2">
@@ -11025,7 +11028,7 @@
         <v>679</v>
       </c>
       <c r="G215" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H215" t="s">
         <v>149</v>
@@ -11034,7 +11037,7 @@
         <v>150</v>
       </c>
       <c r="J215" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L215" s="2" t="s">
         <v>8</v>
@@ -11043,7 +11046,7 @@
         <v>151</v>
       </c>
       <c r="N215" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="216" spans="1:14" x14ac:dyDescent="0.2">
@@ -11063,7 +11066,7 @@
         <v>682</v>
       </c>
       <c r="G216" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H216" t="s">
         <v>149</v>
@@ -11072,7 +11075,7 @@
         <v>150</v>
       </c>
       <c r="J216" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L216" s="2" t="s">
         <v>8</v>
@@ -11081,7 +11084,7 @@
         <v>151</v>
       </c>
       <c r="N216" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.2">
@@ -11101,7 +11104,7 @@
         <v>686</v>
       </c>
       <c r="G217" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H217" t="s">
         <v>149</v>
@@ -11110,7 +11113,7 @@
         <v>150</v>
       </c>
       <c r="J217" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L217" s="2" t="s">
         <v>8</v>
@@ -11119,7 +11122,7 @@
         <v>151</v>
       </c>
       <c r="N217" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.2">
@@ -11139,7 +11142,7 @@
         <v>690</v>
       </c>
       <c r="G218" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H218" t="s">
         <v>149</v>
@@ -11148,7 +11151,7 @@
         <v>150</v>
       </c>
       <c r="J218" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L218" s="2" t="s">
         <v>8</v>
@@ -11157,7 +11160,7 @@
         <v>151</v>
       </c>
       <c r="N218" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="219" spans="1:14" x14ac:dyDescent="0.2">
@@ -11177,7 +11180,7 @@
         <v>694</v>
       </c>
       <c r="G219" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H219" t="s">
         <v>149</v>
@@ -11186,7 +11189,7 @@
         <v>150</v>
       </c>
       <c r="J219" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L219" s="2" t="s">
         <v>8</v>
@@ -11195,7 +11198,7 @@
         <v>151</v>
       </c>
       <c r="N219" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.2">
@@ -11215,7 +11218,7 @@
         <v>698</v>
       </c>
       <c r="G220" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H220" t="s">
         <v>149</v>
@@ -11224,7 +11227,7 @@
         <v>150</v>
       </c>
       <c r="J220" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L220" s="2" t="s">
         <v>8</v>
@@ -11233,7 +11236,7 @@
         <v>151</v>
       </c>
       <c r="N220" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="221" spans="1:14" x14ac:dyDescent="0.2">
@@ -11253,7 +11256,7 @@
         <v>702</v>
       </c>
       <c r="G221" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H221" t="s">
         <v>149</v>
@@ -11262,7 +11265,7 @@
         <v>150</v>
       </c>
       <c r="J221" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L221" s="2" t="s">
         <v>8</v>
@@ -11271,7 +11274,7 @@
         <v>151</v>
       </c>
       <c r="N221" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.2">
@@ -11291,7 +11294,7 @@
         <v>706</v>
       </c>
       <c r="G222" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H222" t="s">
         <v>149</v>
@@ -11300,7 +11303,7 @@
         <v>150</v>
       </c>
       <c r="J222" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L222" s="2" t="s">
         <v>8</v>
@@ -11309,7 +11312,7 @@
         <v>151</v>
       </c>
       <c r="N222" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="223" spans="1:14" x14ac:dyDescent="0.2">
@@ -11329,7 +11332,7 @@
         <v>709</v>
       </c>
       <c r="G223" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H223" t="s">
         <v>149</v>
@@ -11338,7 +11341,7 @@
         <v>150</v>
       </c>
       <c r="J223" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L223" s="2" t="s">
         <v>8</v>
@@ -11347,7 +11350,7 @@
         <v>151</v>
       </c>
       <c r="N223" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.2">
@@ -11367,7 +11370,7 @@
         <v>712</v>
       </c>
       <c r="G224" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H224" t="s">
         <v>149</v>
@@ -11376,7 +11379,7 @@
         <v>150</v>
       </c>
       <c r="J224" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L224" s="2" t="s">
         <v>8</v>
@@ -11385,7 +11388,7 @@
         <v>151</v>
       </c>
       <c r="N224" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.2">
@@ -11405,7 +11408,7 @@
         <v>715</v>
       </c>
       <c r="G225" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H225" t="s">
         <v>149</v>
@@ -11414,7 +11417,7 @@
         <v>150</v>
       </c>
       <c r="J225" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L225" s="2" t="s">
         <v>8</v>
@@ -11423,7 +11426,7 @@
         <v>151</v>
       </c>
       <c r="N225" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.2">
@@ -11443,7 +11446,7 @@
         <v>718</v>
       </c>
       <c r="G226" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H226" t="s">
         <v>149</v>
@@ -11452,7 +11455,7 @@
         <v>150</v>
       </c>
       <c r="J226" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L226" s="2" t="s">
         <v>8</v>
@@ -11461,7 +11464,7 @@
         <v>151</v>
       </c>
       <c r="N226" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.2">
@@ -11481,7 +11484,7 @@
         <v>721</v>
       </c>
       <c r="G227" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H227" t="s">
         <v>149</v>
@@ -11490,7 +11493,7 @@
         <v>150</v>
       </c>
       <c r="J227" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L227" s="2" t="s">
         <v>8</v>
@@ -11499,7 +11502,7 @@
         <v>151</v>
       </c>
       <c r="N227" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.2">
@@ -11519,7 +11522,7 @@
         <v>723</v>
       </c>
       <c r="G228" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H228" t="s">
         <v>149</v>
@@ -11528,7 +11531,7 @@
         <v>150</v>
       </c>
       <c r="J228" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L228" s="2" t="s">
         <v>8</v>
@@ -11537,7 +11540,7 @@
         <v>151</v>
       </c>
       <c r="N228" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.2">
@@ -11557,7 +11560,7 @@
         <v>727</v>
       </c>
       <c r="G229" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H229" t="s">
         <v>149</v>
@@ -11566,7 +11569,7 @@
         <v>150</v>
       </c>
       <c r="J229" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="L229" s="2" t="s">
         <v>8</v>
@@ -11575,7 +11578,7 @@
         <v>151</v>
       </c>
       <c r="N229" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.2">
@@ -11595,7 +11598,7 @@
         <v>730</v>
       </c>
       <c r="G230" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H230" t="s">
         <v>149</v>
@@ -11604,7 +11607,7 @@
         <v>150</v>
       </c>
       <c r="J230" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L230" s="2" t="s">
         <v>8</v>
@@ -11613,7 +11616,7 @@
         <v>151</v>
       </c>
       <c r="N230" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.2">
@@ -11633,7 +11636,7 @@
         <v>732</v>
       </c>
       <c r="G231" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H231" t="s">
         <v>149</v>
@@ -11642,7 +11645,7 @@
         <v>150</v>
       </c>
       <c r="J231" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L231" s="2" t="s">
         <v>8</v>
@@ -11651,7 +11654,7 @@
         <v>151</v>
       </c>
       <c r="N231" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.2">
@@ -11671,7 +11674,7 @@
         <v>735</v>
       </c>
       <c r="G232" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H232" t="s">
         <v>149</v>
@@ -11680,7 +11683,7 @@
         <v>150</v>
       </c>
       <c r="J232" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L232" s="2" t="s">
         <v>8</v>
@@ -11689,7 +11692,7 @@
         <v>151</v>
       </c>
       <c r="N232" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.2">
@@ -11709,7 +11712,7 @@
         <v>738</v>
       </c>
       <c r="G233" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H233" t="s">
         <v>149</v>
@@ -11718,7 +11721,7 @@
         <v>150</v>
       </c>
       <c r="J233" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="L233" s="2" t="s">
         <v>8</v>
@@ -11727,7 +11730,7 @@
         <v>151</v>
       </c>
       <c r="N233" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.2">
@@ -11747,7 +11750,7 @@
         <v>742</v>
       </c>
       <c r="G234" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H234" t="s">
         <v>149</v>
@@ -11756,7 +11759,7 @@
         <v>150</v>
       </c>
       <c r="J234" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L234" s="2" t="s">
         <v>8</v>
@@ -11765,7 +11768,7 @@
         <v>151</v>
       </c>
       <c r="N234" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.2">
@@ -11785,7 +11788,7 @@
         <v>745</v>
       </c>
       <c r="G235" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H235" t="s">
         <v>149</v>
@@ -11794,7 +11797,7 @@
         <v>150</v>
       </c>
       <c r="J235" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L235" s="2" t="s">
         <v>8</v>
@@ -11803,7 +11806,7 @@
         <v>151</v>
       </c>
       <c r="N235" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.2">
@@ -11823,7 +11826,7 @@
         <v>749</v>
       </c>
       <c r="G236" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H236" t="s">
         <v>149</v>
@@ -11832,7 +11835,7 @@
         <v>150</v>
       </c>
       <c r="J236" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L236" s="2" t="s">
         <v>8</v>
@@ -11841,7 +11844,7 @@
         <v>151</v>
       </c>
       <c r="N236" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.2">
@@ -11861,7 +11864,7 @@
         <v>753</v>
       </c>
       <c r="G237" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H237" t="s">
         <v>149</v>
@@ -11870,7 +11873,7 @@
         <v>150</v>
       </c>
       <c r="J237" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L237" s="2" t="s">
         <v>8</v>
@@ -11879,7 +11882,7 @@
         <v>151</v>
       </c>
       <c r="N237" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.2">
@@ -11899,7 +11902,7 @@
         <v>757</v>
       </c>
       <c r="G238" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H238" t="s">
         <v>149</v>
@@ -11908,7 +11911,7 @@
         <v>150</v>
       </c>
       <c r="J238" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="L238" s="2" t="s">
         <v>8</v>
@@ -11917,7 +11920,7 @@
         <v>151</v>
       </c>
       <c r="N238" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.2">
@@ -11937,7 +11940,7 @@
         <v>761</v>
       </c>
       <c r="G239" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H239" t="s">
         <v>149</v>
@@ -11946,7 +11949,7 @@
         <v>150</v>
       </c>
       <c r="J239" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="L239" s="2" t="s">
         <v>8</v>
@@ -11955,7 +11958,7 @@
         <v>151</v>
       </c>
       <c r="N239" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.2">
@@ -11975,7 +11978,7 @@
         <v>764</v>
       </c>
       <c r="G240" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H240" t="s">
         <v>149</v>
@@ -11984,7 +11987,7 @@
         <v>150</v>
       </c>
       <c r="J240" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="L240" s="2" t="s">
         <v>8</v>
@@ -11993,7 +11996,7 @@
         <v>151</v>
       </c>
       <c r="N240" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separar graficos por Atque/defensa corregir2
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\racing-cayma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD36238-4597-4193-B236-124514926DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8997FEE-6B82-4F51-AE3C-7B662B153CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2441,7 +2441,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:N240" totalsRowShown="0">
-  <autoFilter ref="A1:N240" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
+  <autoFilter ref="A1:N240" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Ocasió"/>
+        <filter val="Ocasión"/>
+        <filter val="Ocasión rival"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Event"/>
     <tableColumn id="2" xr3:uid="{4A939A0F-B787-4665-B94F-35DE80E0B243}" name="start_time"/>
@@ -2752,7 +2760,7 @@
   <dimension ref="A1:N240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2810,7 +2818,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -2846,7 +2854,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2885,7 +2893,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2924,7 +2932,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2960,7 +2968,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2999,7 +3007,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3038,7 +3046,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3119,7 +3127,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3158,7 +3166,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3197,7 +3205,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3236,7 +3244,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -3272,7 +3280,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3311,7 +3319,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3350,7 +3358,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -3428,7 +3436,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3467,7 +3475,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -3506,7 +3514,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3545,7 +3553,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -3584,7 +3592,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3623,7 +3631,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -3662,7 +3670,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3698,7 +3706,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -3737,7 +3745,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -3776,7 +3784,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -3854,7 +3862,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -3893,7 +3901,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -3932,7 +3940,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -3971,7 +3979,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -4007,7 +4015,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -4046,7 +4054,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -4082,7 +4090,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -4121,7 +4129,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -4160,7 +4168,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -4199,7 +4207,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -4238,7 +4246,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>152</v>
       </c>
@@ -4274,7 +4282,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -4313,7 +4321,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -4352,7 +4360,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -4391,7 +4399,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -4430,7 +4438,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -4469,7 +4477,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -4508,7 +4516,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -4547,7 +4555,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -4586,7 +4594,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -4625,7 +4633,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -4664,7 +4672,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -4703,7 +4711,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -4781,7 +4789,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -4820,7 +4828,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -4859,7 +4867,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -4898,7 +4906,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -4937,7 +4945,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -4976,7 +4984,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -5015,7 +5023,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -5054,7 +5062,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -5093,7 +5101,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -5132,7 +5140,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -5171,7 +5179,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -5210,7 +5218,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -5246,7 +5254,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -5285,7 +5293,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -5324,7 +5332,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -5363,7 +5371,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -5402,7 +5410,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -5441,7 +5449,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -5480,7 +5488,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>152</v>
       </c>
@@ -5555,7 +5563,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -5594,7 +5602,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -5633,7 +5641,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -5672,7 +5680,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -5711,7 +5719,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -5750,7 +5758,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -5789,7 +5797,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -5828,7 +5836,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -5867,7 +5875,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -5906,7 +5914,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -5945,7 +5953,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -5984,7 +5992,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -6023,7 +6031,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -6062,7 +6070,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>152</v>
       </c>
@@ -6098,7 +6106,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -6137,7 +6145,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>15</v>
       </c>
@@ -6176,7 +6184,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -6215,7 +6223,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -6254,7 +6262,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -6293,7 +6301,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -6332,7 +6340,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -6371,7 +6379,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -6410,7 +6418,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -6449,7 +6457,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -6488,7 +6496,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -6527,7 +6535,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>152</v>
       </c>
@@ -6644,7 +6652,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -6683,7 +6691,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -6722,7 +6730,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -6761,7 +6769,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -6820,7 +6828,7 @@
         <v>427</v>
       </c>
       <c r="G105" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H105" t="s">
         <v>149</v>
@@ -6842,7 +6850,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -6881,7 +6889,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -6920,7 +6928,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>1</v>
       </c>
@@ -6998,7 +7006,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>3</v>
       </c>
@@ -7037,7 +7045,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>15</v>
       </c>
@@ -7076,7 +7084,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -7115,7 +7123,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -7154,7 +7162,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -7193,7 +7201,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>3</v>
       </c>
@@ -7232,7 +7240,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>15</v>
       </c>
@@ -7271,7 +7279,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -7310,7 +7318,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>152</v>
       </c>
@@ -7346,7 +7354,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>3</v>
       </c>
@@ -7385,7 +7393,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>17</v>
       </c>
@@ -7424,7 +7432,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>1</v>
       </c>
@@ -7463,7 +7471,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -7502,7 +7510,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>17</v>
       </c>
@@ -7541,7 +7549,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>1</v>
       </c>
@@ -7580,7 +7588,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>17</v>
       </c>
@@ -7619,7 +7627,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>1</v>
       </c>
@@ -7658,7 +7666,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>15</v>
       </c>
@@ -7697,7 +7705,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>1</v>
       </c>
@@ -7736,7 +7744,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>15</v>
       </c>
@@ -7814,7 +7822,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>1</v>
       </c>
@@ -7853,7 +7861,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>17</v>
       </c>
@@ -7892,7 +7900,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>15</v>
       </c>
@@ -7931,7 +7939,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -7970,7 +7978,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>3</v>
       </c>
@@ -8009,7 +8017,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>428</v>
       </c>
@@ -8047,7 +8055,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>428</v>
       </c>
@@ -8085,7 +8093,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>428</v>
       </c>
@@ -8123,7 +8131,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>428</v>
       </c>
@@ -8161,7 +8169,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>428</v>
       </c>
@@ -8199,7 +8207,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>428</v>
       </c>
@@ -8237,7 +8245,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>428</v>
       </c>
@@ -8275,7 +8283,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>428</v>
       </c>
@@ -8313,7 +8321,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>428</v>
       </c>
@@ -8351,7 +8359,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>428</v>
       </c>
@@ -8389,7 +8397,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>428</v>
       </c>
@@ -8427,7 +8435,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>428</v>
       </c>
@@ -8465,7 +8473,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>428</v>
       </c>
@@ -8503,7 +8511,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>428</v>
       </c>
@@ -8541,7 +8549,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>428</v>
       </c>
@@ -8579,7 +8587,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>428</v>
       </c>
@@ -8617,7 +8625,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>428</v>
       </c>
@@ -8655,7 +8663,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>428</v>
       </c>
@@ -8693,7 +8701,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>428</v>
       </c>
@@ -8731,7 +8739,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>428</v>
       </c>
@@ -8769,7 +8777,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>428</v>
       </c>
@@ -8807,7 +8815,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>428</v>
       </c>
@@ -8845,7 +8853,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>428</v>
       </c>
@@ -8883,7 +8891,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>428</v>
       </c>
@@ -8921,7 +8929,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>428</v>
       </c>
@@ -8959,7 +8967,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>428</v>
       </c>
@@ -8997,7 +9005,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>428</v>
       </c>
@@ -9035,7 +9043,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>428</v>
       </c>
@@ -9073,7 +9081,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>428</v>
       </c>
@@ -9111,7 +9119,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>428</v>
       </c>
@@ -9149,7 +9157,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>428</v>
       </c>
@@ -9187,7 +9195,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>428</v>
       </c>
@@ -9225,7 +9233,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>428</v>
       </c>
@@ -9263,7 +9271,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>428</v>
       </c>
@@ -9301,7 +9309,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>428</v>
       </c>
@@ -9339,7 +9347,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>428</v>
       </c>
@@ -9377,7 +9385,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>428</v>
       </c>
@@ -9415,7 +9423,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>428</v>
       </c>
@@ -9453,7 +9461,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>428</v>
       </c>
@@ -9491,7 +9499,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>428</v>
       </c>
@@ -9529,7 +9537,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>428</v>
       </c>
@@ -9567,7 +9575,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>428</v>
       </c>
@@ -9605,7 +9613,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>428</v>
       </c>
@@ -9643,7 +9651,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>428</v>
       </c>
@@ -9681,7 +9689,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>428</v>
       </c>
@@ -9719,7 +9727,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>428</v>
       </c>
@@ -9757,7 +9765,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>428</v>
       </c>
@@ -9795,7 +9803,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>428</v>
       </c>
@@ -9833,7 +9841,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>428</v>
       </c>
@@ -9871,7 +9879,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>428</v>
       </c>
@@ -9909,7 +9917,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>428</v>
       </c>
@@ -9947,7 +9955,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>428</v>
       </c>
@@ -9985,7 +9993,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>428</v>
       </c>
@@ -10023,7 +10031,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>428</v>
       </c>
@@ -10061,7 +10069,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>428</v>
       </c>
@@ -10099,7 +10107,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>428</v>
       </c>
@@ -10137,7 +10145,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>428</v>
       </c>
@@ -10175,7 +10183,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>428</v>
       </c>
@@ -10213,7 +10221,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>428</v>
       </c>
@@ -10251,7 +10259,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>428</v>
       </c>
@@ -10289,7 +10297,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>428</v>
       </c>
@@ -10327,7 +10335,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>428</v>
       </c>
@@ -10365,7 +10373,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>428</v>
       </c>
@@ -10403,7 +10411,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>428</v>
       </c>
@@ -10441,7 +10449,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>428</v>
       </c>
@@ -10479,7 +10487,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>428</v>
       </c>
@@ -10517,7 +10525,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>428</v>
       </c>
@@ -10555,7 +10563,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>428</v>
       </c>
@@ -10593,7 +10601,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>428</v>
       </c>
@@ -10631,7 +10639,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>428</v>
       </c>
@@ -10669,7 +10677,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>428</v>
       </c>
@@ -10707,7 +10715,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>428</v>
       </c>
@@ -10745,7 +10753,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>428</v>
       </c>
@@ -10783,7 +10791,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>428</v>
       </c>
@@ -10821,7 +10829,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>428</v>
       </c>
@@ -10859,7 +10867,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>428</v>
       </c>
@@ -10897,7 +10905,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>428</v>
       </c>
@@ -10935,7 +10943,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>428</v>
       </c>
@@ -10973,7 +10981,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>428</v>
       </c>
@@ -11011,7 +11019,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>428</v>
       </c>
@@ -11049,7 +11057,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>428</v>
       </c>
@@ -11087,7 +11095,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>428</v>
       </c>
@@ -11125,7 +11133,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>428</v>
       </c>
@@ -11163,7 +11171,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>428</v>
       </c>
@@ -11201,7 +11209,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>428</v>
       </c>
@@ -11239,7 +11247,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>428</v>
       </c>
@@ -11277,7 +11285,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>428</v>
       </c>
@@ -11315,7 +11323,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>428</v>
       </c>
@@ -11353,7 +11361,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>428</v>
       </c>
@@ -11391,7 +11399,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>428</v>
       </c>
@@ -11429,7 +11437,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>428</v>
       </c>
@@ -11467,7 +11475,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>428</v>
       </c>
@@ -11505,7 +11513,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>428</v>
       </c>
@@ -11543,7 +11551,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>428</v>
       </c>
@@ -11581,7 +11589,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>428</v>
       </c>
@@ -11619,7 +11627,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>428</v>
       </c>
@@ -11657,7 +11665,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>428</v>
       </c>
@@ -11695,7 +11703,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>428</v>
       </c>
@@ -11733,7 +11741,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>428</v>
       </c>
@@ -11771,7 +11779,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>428</v>
       </c>
@@ -11809,7 +11817,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>428</v>
       </c>
@@ -11847,7 +11855,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>428</v>
       </c>
@@ -11885,7 +11893,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>428</v>
       </c>
@@ -11923,7 +11931,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>428</v>
       </c>
@@ -11961,7 +11969,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>428</v>
       </c>

</xml_diff>

<commit_message>
update pases excel event
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\racing-cayma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D522492-9215-4218-B90C-370577AB7FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C05A21C-744C-4EBB-A230-0D9304B74434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="1213">
   <si>
     <t>XY</t>
   </si>
@@ -3650,6 +3650,15 @@
   </si>
   <si>
     <t>67;70 78;100</t>
+  </si>
+  <si>
+    <t>Desconocido</t>
+  </si>
+  <si>
+    <t>Ampuero</t>
+  </si>
+  <si>
+    <t>desconocido</t>
   </si>
 </sst>
 </file>
@@ -4047,7 +4056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77939FC4-FC73-4262-977F-310955BE7B1D}">
   <dimension ref="A1:N367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C227" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C121" workbookViewId="0">
       <selection activeCell="J136" sqref="J136:J367"/>
     </sheetView>
   </sheetViews>
@@ -9331,7 +9340,7 @@
         <v>150</v>
       </c>
       <c r="J136" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L136" s="2" t="s">
         <v>8</v>
@@ -9369,7 +9378,7 @@
         <v>150</v>
       </c>
       <c r="J137" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L137" s="2" t="s">
         <v>8</v>
@@ -9407,7 +9416,7 @@
         <v>150</v>
       </c>
       <c r="J138" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L138" s="2" t="s">
         <v>8</v>
@@ -9445,7 +9454,7 @@
         <v>150</v>
       </c>
       <c r="J139" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L139" s="2" t="s">
         <v>8</v>
@@ -9483,7 +9492,7 @@
         <v>150</v>
       </c>
       <c r="J140" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>8</v>
@@ -9521,7 +9530,7 @@
         <v>150</v>
       </c>
       <c r="J141" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L141" s="2" t="s">
         <v>8</v>
@@ -9559,7 +9568,7 @@
         <v>150</v>
       </c>
       <c r="J142" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L142" s="2" t="s">
         <v>8</v>
@@ -9597,7 +9606,7 @@
         <v>150</v>
       </c>
       <c r="J143" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L143" s="2" t="s">
         <v>8</v>
@@ -9635,7 +9644,7 @@
         <v>150</v>
       </c>
       <c r="J144" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L144" s="2" t="s">
         <v>8</v>
@@ -9673,7 +9682,7 @@
         <v>150</v>
       </c>
       <c r="J145" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L145" s="2" t="s">
         <v>8</v>
@@ -9711,7 +9720,7 @@
         <v>150</v>
       </c>
       <c r="J146" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L146" s="2" t="s">
         <v>8</v>
@@ -9749,7 +9758,7 @@
         <v>150</v>
       </c>
       <c r="J147" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L147" s="2" t="s">
         <v>8</v>
@@ -9787,7 +9796,7 @@
         <v>150</v>
       </c>
       <c r="J148" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L148" s="2" t="s">
         <v>8</v>
@@ -9825,7 +9834,7 @@
         <v>150</v>
       </c>
       <c r="J149" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L149" s="2" t="s">
         <v>8</v>
@@ -9863,7 +9872,7 @@
         <v>150</v>
       </c>
       <c r="J150" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L150" s="2" t="s">
         <v>8</v>
@@ -9901,7 +9910,7 @@
         <v>150</v>
       </c>
       <c r="J151" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L151" s="2" t="s">
         <v>8</v>
@@ -9939,7 +9948,7 @@
         <v>150</v>
       </c>
       <c r="J152" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L152" s="2" t="s">
         <v>8</v>
@@ -9977,7 +9986,7 @@
         <v>150</v>
       </c>
       <c r="J153" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L153" s="2" t="s">
         <v>8</v>
@@ -10015,7 +10024,7 @@
         <v>150</v>
       </c>
       <c r="J154" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L154" s="2" t="s">
         <v>8</v>
@@ -10053,7 +10062,7 @@
         <v>150</v>
       </c>
       <c r="J155" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L155" s="2" t="s">
         <v>8</v>
@@ -10091,7 +10100,7 @@
         <v>150</v>
       </c>
       <c r="J156" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L156" s="2" t="s">
         <v>8</v>
@@ -10129,7 +10138,7 @@
         <v>150</v>
       </c>
       <c r="J157" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L157" s="2" t="s">
         <v>8</v>
@@ -10167,7 +10176,7 @@
         <v>150</v>
       </c>
       <c r="J158" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L158" s="2" t="s">
         <v>8</v>
@@ -10205,7 +10214,7 @@
         <v>150</v>
       </c>
       <c r="J159" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L159" s="2" t="s">
         <v>8</v>
@@ -10243,7 +10252,7 @@
         <v>150</v>
       </c>
       <c r="J160" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L160" s="2" t="s">
         <v>8</v>
@@ -10281,7 +10290,7 @@
         <v>150</v>
       </c>
       <c r="J161" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L161" s="2" t="s">
         <v>8</v>
@@ -10319,7 +10328,7 @@
         <v>150</v>
       </c>
       <c r="J162" t="s">
-        <v>762</v>
+        <v>1211</v>
       </c>
       <c r="L162" s="2" t="s">
         <v>8</v>
@@ -10357,7 +10366,7 @@
         <v>150</v>
       </c>
       <c r="J163" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L163" s="2" t="s">
         <v>8</v>
@@ -10395,7 +10404,7 @@
         <v>150</v>
       </c>
       <c r="J164" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L164" s="2" t="s">
         <v>8</v>
@@ -10433,7 +10442,7 @@
         <v>150</v>
       </c>
       <c r="J165" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L165" s="2" t="s">
         <v>8</v>
@@ -10471,7 +10480,7 @@
         <v>150</v>
       </c>
       <c r="J166" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L166" s="2" t="s">
         <v>8</v>
@@ -10509,7 +10518,7 @@
         <v>150</v>
       </c>
       <c r="J167" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L167" s="2" t="s">
         <v>8</v>
@@ -10547,7 +10556,7 @@
         <v>150</v>
       </c>
       <c r="J168" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L168" s="2" t="s">
         <v>8</v>
@@ -10585,7 +10594,7 @@
         <v>150</v>
       </c>
       <c r="J169" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L169" s="2" t="s">
         <v>8</v>
@@ -10623,7 +10632,7 @@
         <v>150</v>
       </c>
       <c r="J170" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L170" s="2" t="s">
         <v>8</v>
@@ -10661,7 +10670,7 @@
         <v>150</v>
       </c>
       <c r="J171" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L171" s="2" t="s">
         <v>8</v>
@@ -10699,7 +10708,7 @@
         <v>150</v>
       </c>
       <c r="J172" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L172" s="2" t="s">
         <v>8</v>
@@ -10737,7 +10746,7 @@
         <v>150</v>
       </c>
       <c r="J173" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L173" s="2" t="s">
         <v>8</v>
@@ -10775,7 +10784,7 @@
         <v>150</v>
       </c>
       <c r="J174" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L174" s="2" t="s">
         <v>8</v>
@@ -10813,7 +10822,7 @@
         <v>150</v>
       </c>
       <c r="J175" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L175" s="2" t="s">
         <v>8</v>
@@ -10851,7 +10860,7 @@
         <v>150</v>
       </c>
       <c r="J176" t="s">
-        <v>762</v>
+        <v>1211</v>
       </c>
       <c r="L176" s="2" t="s">
         <v>8</v>
@@ -10889,7 +10898,7 @@
         <v>150</v>
       </c>
       <c r="J177" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L177" s="2" t="s">
         <v>8</v>
@@ -10927,7 +10936,7 @@
         <v>150</v>
       </c>
       <c r="J178" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L178" s="2" t="s">
         <v>8</v>
@@ -10965,7 +10974,7 @@
         <v>150</v>
       </c>
       <c r="J179" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L179" s="2" t="s">
         <v>8</v>
@@ -11003,7 +11012,7 @@
         <v>150</v>
       </c>
       <c r="J180" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L180" s="2" t="s">
         <v>8</v>
@@ -11041,7 +11050,7 @@
         <v>150</v>
       </c>
       <c r="J181" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L181" s="2" t="s">
         <v>8</v>
@@ -11079,7 +11088,7 @@
         <v>150</v>
       </c>
       <c r="J182" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L182" s="2" t="s">
         <v>8</v>
@@ -11117,7 +11126,7 @@
         <v>150</v>
       </c>
       <c r="J183" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L183" s="2" t="s">
         <v>8</v>
@@ -11155,7 +11164,7 @@
         <v>150</v>
       </c>
       <c r="J184" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L184" s="2" t="s">
         <v>8</v>
@@ -11193,7 +11202,7 @@
         <v>150</v>
       </c>
       <c r="J185" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L185" s="2" t="s">
         <v>8</v>
@@ -11231,7 +11240,7 @@
         <v>150</v>
       </c>
       <c r="J186" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L186" s="2" t="s">
         <v>8</v>
@@ -11269,7 +11278,7 @@
         <v>150</v>
       </c>
       <c r="J187" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L187" s="2" t="s">
         <v>8</v>
@@ -11307,7 +11316,7 @@
         <v>150</v>
       </c>
       <c r="J188" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L188" s="2" t="s">
         <v>8</v>
@@ -11345,7 +11354,7 @@
         <v>150</v>
       </c>
       <c r="J189" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L189" s="2" t="s">
         <v>8</v>
@@ -11383,7 +11392,7 @@
         <v>150</v>
       </c>
       <c r="J190" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L190" s="2" t="s">
         <v>8</v>
@@ -11421,7 +11430,7 @@
         <v>150</v>
       </c>
       <c r="J191" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L191" s="2" t="s">
         <v>8</v>
@@ -11459,7 +11468,7 @@
         <v>150</v>
       </c>
       <c r="J192" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L192" s="2" t="s">
         <v>8</v>
@@ -11497,7 +11506,7 @@
         <v>150</v>
       </c>
       <c r="J193" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L193" s="2" t="s">
         <v>8</v>
@@ -11535,7 +11544,7 @@
         <v>150</v>
       </c>
       <c r="J194" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L194" s="2" t="s">
         <v>8</v>
@@ -11573,7 +11582,7 @@
         <v>150</v>
       </c>
       <c r="J195" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L195" s="2" t="s">
         <v>8</v>
@@ -11611,7 +11620,7 @@
         <v>150</v>
       </c>
       <c r="J196" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L196" s="2" t="s">
         <v>8</v>
@@ -11649,7 +11658,7 @@
         <v>150</v>
       </c>
       <c r="J197" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L197" s="2" t="s">
         <v>8</v>
@@ -11687,7 +11696,7 @@
         <v>150</v>
       </c>
       <c r="J198" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L198" s="2" t="s">
         <v>8</v>
@@ -11725,7 +11734,7 @@
         <v>150</v>
       </c>
       <c r="J199" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L199" s="2" t="s">
         <v>8</v>
@@ -11763,7 +11772,7 @@
         <v>150</v>
       </c>
       <c r="J200" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L200" s="2" t="s">
         <v>8</v>
@@ -11801,7 +11810,7 @@
         <v>150</v>
       </c>
       <c r="J201" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L201" s="2" t="s">
         <v>8</v>
@@ -11839,7 +11848,7 @@
         <v>150</v>
       </c>
       <c r="J202" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L202" s="2" t="s">
         <v>8</v>
@@ -11877,7 +11886,7 @@
         <v>150</v>
       </c>
       <c r="J203" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L203" s="2" t="s">
         <v>8</v>
@@ -11915,7 +11924,7 @@
         <v>150</v>
       </c>
       <c r="J204" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L204" s="2" t="s">
         <v>8</v>
@@ -11953,7 +11962,7 @@
         <v>150</v>
       </c>
       <c r="J205" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L205" s="2" t="s">
         <v>8</v>
@@ -11991,7 +12000,7 @@
         <v>150</v>
       </c>
       <c r="J206" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L206" s="2" t="s">
         <v>8</v>
@@ -12029,7 +12038,7 @@
         <v>150</v>
       </c>
       <c r="J207" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L207" s="2" t="s">
         <v>8</v>
@@ -12067,7 +12076,7 @@
         <v>150</v>
       </c>
       <c r="J208" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L208" s="2" t="s">
         <v>8</v>
@@ -12105,7 +12114,7 @@
         <v>150</v>
       </c>
       <c r="J209" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L209" s="2" t="s">
         <v>8</v>
@@ -12143,7 +12152,7 @@
         <v>150</v>
       </c>
       <c r="J210" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L210" s="2" t="s">
         <v>8</v>
@@ -12181,7 +12190,7 @@
         <v>150</v>
       </c>
       <c r="J211" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L211" s="2" t="s">
         <v>8</v>
@@ -12219,7 +12228,7 @@
         <v>150</v>
       </c>
       <c r="J212" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L212" s="2" t="s">
         <v>8</v>
@@ -12257,7 +12266,7 @@
         <v>150</v>
       </c>
       <c r="J213" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L213" s="2" t="s">
         <v>8</v>
@@ -12295,7 +12304,7 @@
         <v>150</v>
       </c>
       <c r="J214" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L214" s="2" t="s">
         <v>8</v>
@@ -12333,7 +12342,7 @@
         <v>150</v>
       </c>
       <c r="J215" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L215" s="2" t="s">
         <v>8</v>
@@ -12371,7 +12380,7 @@
         <v>150</v>
       </c>
       <c r="J216" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L216" s="2" t="s">
         <v>8</v>
@@ -12409,7 +12418,7 @@
         <v>150</v>
       </c>
       <c r="J217" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L217" s="2" t="s">
         <v>8</v>
@@ -12447,7 +12456,7 @@
         <v>150</v>
       </c>
       <c r="J218" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L218" s="2" t="s">
         <v>8</v>
@@ -12485,7 +12494,7 @@
         <v>150</v>
       </c>
       <c r="J219" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L219" s="2" t="s">
         <v>8</v>
@@ -12523,7 +12532,7 @@
         <v>150</v>
       </c>
       <c r="J220" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L220" s="2" t="s">
         <v>8</v>
@@ -12561,7 +12570,7 @@
         <v>150</v>
       </c>
       <c r="J221" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L221" s="2" t="s">
         <v>8</v>
@@ -12599,7 +12608,7 @@
         <v>150</v>
       </c>
       <c r="J222" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L222" s="2" t="s">
         <v>8</v>
@@ -12637,7 +12646,7 @@
         <v>150</v>
       </c>
       <c r="J223" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L223" s="2" t="s">
         <v>8</v>
@@ -12675,7 +12684,7 @@
         <v>150</v>
       </c>
       <c r="J224" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L224" s="2" t="s">
         <v>8</v>
@@ -12713,7 +12722,7 @@
         <v>150</v>
       </c>
       <c r="J225" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L225" s="2" t="s">
         <v>8</v>
@@ -12751,7 +12760,7 @@
         <v>150</v>
       </c>
       <c r="J226" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L226" s="2" t="s">
         <v>8</v>
@@ -12789,7 +12798,7 @@
         <v>150</v>
       </c>
       <c r="J227" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L227" s="2" t="s">
         <v>8</v>
@@ -12827,7 +12836,7 @@
         <v>150</v>
       </c>
       <c r="J228" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L228" s="2" t="s">
         <v>8</v>
@@ -12865,7 +12874,7 @@
         <v>150</v>
       </c>
       <c r="J229" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L229" s="2" t="s">
         <v>8</v>
@@ -12903,7 +12912,7 @@
         <v>150</v>
       </c>
       <c r="J230" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L230" s="2" t="s">
         <v>8</v>
@@ -12941,7 +12950,7 @@
         <v>150</v>
       </c>
       <c r="J231" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L231" s="2" t="s">
         <v>8</v>
@@ -12979,7 +12988,7 @@
         <v>150</v>
       </c>
       <c r="J232" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L232" s="2" t="s">
         <v>8</v>
@@ -13017,7 +13026,7 @@
         <v>150</v>
       </c>
       <c r="J233" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L233" s="2" t="s">
         <v>8</v>
@@ -13055,7 +13064,7 @@
         <v>150</v>
       </c>
       <c r="J234" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L234" s="2" t="s">
         <v>8</v>
@@ -13093,7 +13102,7 @@
         <v>150</v>
       </c>
       <c r="J235" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L235" s="2" t="s">
         <v>8</v>
@@ -13131,7 +13140,7 @@
         <v>150</v>
       </c>
       <c r="J236" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L236" s="2" t="s">
         <v>8</v>
@@ -13169,7 +13178,7 @@
         <v>150</v>
       </c>
       <c r="J237" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L237" s="2" t="s">
         <v>8</v>
@@ -13207,7 +13216,7 @@
         <v>150</v>
       </c>
       <c r="J238" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L238" s="2" t="s">
         <v>8</v>
@@ -13245,7 +13254,7 @@
         <v>150</v>
       </c>
       <c r="J239" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L239" s="2" t="s">
         <v>8</v>
@@ -13283,7 +13292,7 @@
         <v>150</v>
       </c>
       <c r="J240" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L240" s="2" t="s">
         <v>8</v>
@@ -13321,7 +13330,7 @@
         <v>150</v>
       </c>
       <c r="J241" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L241" s="2" t="s">
         <v>8</v>
@@ -13359,7 +13368,7 @@
         <v>150</v>
       </c>
       <c r="J242" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L242" s="2" t="s">
         <v>8</v>
@@ -13397,7 +13406,7 @@
         <v>150</v>
       </c>
       <c r="J243" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L243" s="2" t="s">
         <v>8</v>
@@ -13435,7 +13444,7 @@
         <v>150</v>
       </c>
       <c r="J244" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L244" s="2" t="s">
         <v>8</v>
@@ -13473,7 +13482,7 @@
         <v>150</v>
       </c>
       <c r="J245" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L245" s="2" t="s">
         <v>8</v>
@@ -13511,7 +13520,7 @@
         <v>150</v>
       </c>
       <c r="J246" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L246" s="2" t="s">
         <v>8</v>
@@ -13549,7 +13558,7 @@
         <v>150</v>
       </c>
       <c r="J247" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L247" s="2" t="s">
         <v>8</v>
@@ -13587,7 +13596,7 @@
         <v>150</v>
       </c>
       <c r="J248" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L248" s="2" t="s">
         <v>8</v>
@@ -13625,7 +13634,7 @@
         <v>150</v>
       </c>
       <c r="J249" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L249" s="2" t="s">
         <v>8</v>
@@ -13663,7 +13672,7 @@
         <v>150</v>
       </c>
       <c r="J250" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L250" s="2" t="s">
         <v>8</v>
@@ -13701,7 +13710,7 @@
         <v>150</v>
       </c>
       <c r="J251" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L251" s="2" t="s">
         <v>8</v>
@@ -13739,7 +13748,7 @@
         <v>150</v>
       </c>
       <c r="J252" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L252" s="2" t="s">
         <v>8</v>
@@ -13777,7 +13786,7 @@
         <v>150</v>
       </c>
       <c r="J253" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L253" s="2" t="s">
         <v>8</v>
@@ -13813,7 +13822,7 @@
         <v>150</v>
       </c>
       <c r="J254" s="3" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L254" s="2" t="s">
         <v>8</v>
@@ -13851,7 +13860,7 @@
         <v>150</v>
       </c>
       <c r="J255" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L255" s="2" t="s">
         <v>8</v>
@@ -13889,7 +13898,7 @@
         <v>150</v>
       </c>
       <c r="J256" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L256" s="2" t="s">
         <v>8</v>
@@ -13927,7 +13936,7 @@
         <v>150</v>
       </c>
       <c r="J257" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L257" s="2" t="s">
         <v>8</v>
@@ -13965,7 +13974,7 @@
         <v>150</v>
       </c>
       <c r="J258" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L258" s="2" t="s">
         <v>8</v>
@@ -14003,7 +14012,7 @@
         <v>150</v>
       </c>
       <c r="J259" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L259" s="2" t="s">
         <v>8</v>
@@ -14041,7 +14050,7 @@
         <v>150</v>
       </c>
       <c r="J260" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L260" s="2" t="s">
         <v>8</v>
@@ -14079,7 +14088,7 @@
         <v>150</v>
       </c>
       <c r="J261" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L261" s="2" t="s">
         <v>8</v>
@@ -14117,7 +14126,7 @@
         <v>150</v>
       </c>
       <c r="J262" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L262" s="2" t="s">
         <v>8</v>
@@ -14155,7 +14164,7 @@
         <v>150</v>
       </c>
       <c r="J263" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L263" s="2" t="s">
         <v>8</v>
@@ -14193,7 +14202,7 @@
         <v>150</v>
       </c>
       <c r="J264" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L264" s="2" t="s">
         <v>8</v>
@@ -14231,7 +14240,7 @@
         <v>150</v>
       </c>
       <c r="J265" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L265" s="2" t="s">
         <v>8</v>
@@ -14269,7 +14278,7 @@
         <v>150</v>
       </c>
       <c r="J266" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L266" s="2" t="s">
         <v>8</v>
@@ -14307,7 +14316,7 @@
         <v>150</v>
       </c>
       <c r="J267" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L267" s="2" t="s">
         <v>8</v>
@@ -14345,7 +14354,7 @@
         <v>150</v>
       </c>
       <c r="J268" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L268" s="2" t="s">
         <v>8</v>
@@ -14383,7 +14392,7 @@
         <v>150</v>
       </c>
       <c r="J269" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L269" s="2" t="s">
         <v>8</v>
@@ -14421,7 +14430,7 @@
         <v>150</v>
       </c>
       <c r="J270" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L270" s="2" t="s">
         <v>8</v>
@@ -14459,7 +14468,7 @@
         <v>150</v>
       </c>
       <c r="J271" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L271" s="2" t="s">
         <v>8</v>
@@ -14497,7 +14506,7 @@
         <v>150</v>
       </c>
       <c r="J272" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L272" s="2" t="s">
         <v>8</v>
@@ -14535,7 +14544,7 @@
         <v>150</v>
       </c>
       <c r="J273" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L273" s="2" t="s">
         <v>8</v>
@@ -14573,7 +14582,7 @@
         <v>150</v>
       </c>
       <c r="J274" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L274" s="2" t="s">
         <v>8</v>
@@ -14611,7 +14620,7 @@
         <v>150</v>
       </c>
       <c r="J275" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L275" s="2" t="s">
         <v>8</v>
@@ -14649,7 +14658,7 @@
         <v>150</v>
       </c>
       <c r="J276" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L276" s="2" t="s">
         <v>8</v>
@@ -14687,7 +14696,7 @@
         <v>150</v>
       </c>
       <c r="J277" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L277" s="2" t="s">
         <v>8</v>
@@ -14725,7 +14734,7 @@
         <v>150</v>
       </c>
       <c r="J278" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L278" s="2" t="s">
         <v>8</v>
@@ -14763,7 +14772,7 @@
         <v>150</v>
       </c>
       <c r="J279" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L279" s="2" t="s">
         <v>8</v>
@@ -14801,7 +14810,7 @@
         <v>150</v>
       </c>
       <c r="J280" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L280" s="2" t="s">
         <v>8</v>
@@ -14839,7 +14848,7 @@
         <v>150</v>
       </c>
       <c r="J281" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L281" s="2" t="s">
         <v>8</v>
@@ -14877,7 +14886,7 @@
         <v>150</v>
       </c>
       <c r="J282" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L282" s="2" t="s">
         <v>8</v>
@@ -14915,7 +14924,7 @@
         <v>150</v>
       </c>
       <c r="J283" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L283" s="2" t="s">
         <v>8</v>
@@ -14953,7 +14962,7 @@
         <v>150</v>
       </c>
       <c r="J284" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L284" s="2" t="s">
         <v>8</v>
@@ -14991,7 +15000,7 @@
         <v>150</v>
       </c>
       <c r="J285" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L285" s="2" t="s">
         <v>8</v>
@@ -15029,7 +15038,7 @@
         <v>150</v>
       </c>
       <c r="J286" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L286" s="2" t="s">
         <v>8</v>
@@ -15067,7 +15076,7 @@
         <v>150</v>
       </c>
       <c r="J287" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L287" s="2" t="s">
         <v>8</v>
@@ -15105,7 +15114,7 @@
         <v>150</v>
       </c>
       <c r="J288" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L288" s="2" t="s">
         <v>8</v>
@@ -15143,7 +15152,7 @@
         <v>150</v>
       </c>
       <c r="J289" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L289" s="2" t="s">
         <v>8</v>
@@ -15181,7 +15190,7 @@
         <v>150</v>
       </c>
       <c r="J290" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L290" s="2" t="s">
         <v>8</v>
@@ -15219,7 +15228,7 @@
         <v>150</v>
       </c>
       <c r="J291" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L291" s="2" t="s">
         <v>8</v>
@@ -15257,7 +15266,7 @@
         <v>150</v>
       </c>
       <c r="J292" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L292" s="2" t="s">
         <v>8</v>
@@ -15295,7 +15304,7 @@
         <v>150</v>
       </c>
       <c r="J293" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L293" s="2" t="s">
         <v>8</v>
@@ -15333,7 +15342,7 @@
         <v>150</v>
       </c>
       <c r="J294" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L294" s="2" t="s">
         <v>8</v>
@@ -15371,7 +15380,7 @@
         <v>150</v>
       </c>
       <c r="J295" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L295" s="2" t="s">
         <v>8</v>
@@ -15409,7 +15418,7 @@
         <v>150</v>
       </c>
       <c r="J296" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L296" s="2" t="s">
         <v>8</v>
@@ -15447,7 +15456,7 @@
         <v>150</v>
       </c>
       <c r="J297" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L297" s="2" t="s">
         <v>8</v>
@@ -15485,7 +15494,7 @@
         <v>150</v>
       </c>
       <c r="J298" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L298" s="2" t="s">
         <v>8</v>
@@ -15523,7 +15532,7 @@
         <v>150</v>
       </c>
       <c r="J299" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L299" s="2" t="s">
         <v>8</v>
@@ -15561,7 +15570,7 @@
         <v>150</v>
       </c>
       <c r="J300" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L300" s="2" t="s">
         <v>8</v>
@@ -15599,7 +15608,7 @@
         <v>150</v>
       </c>
       <c r="J301" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L301" s="2" t="s">
         <v>8</v>
@@ -15637,7 +15646,7 @@
         <v>150</v>
       </c>
       <c r="J302" t="s">
-        <v>762</v>
+        <v>1211</v>
       </c>
       <c r="L302" s="2" t="s">
         <v>8</v>
@@ -15675,7 +15684,7 @@
         <v>150</v>
       </c>
       <c r="J303" t="s">
-        <v>762</v>
+        <v>1211</v>
       </c>
       <c r="L303" s="2" t="s">
         <v>8</v>
@@ -15713,7 +15722,7 @@
         <v>150</v>
       </c>
       <c r="J304" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L304" s="2" t="s">
         <v>8</v>
@@ -15751,7 +15760,7 @@
         <v>150</v>
       </c>
       <c r="J305" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L305" s="2" t="s">
         <v>8</v>
@@ -15789,7 +15798,7 @@
         <v>150</v>
       </c>
       <c r="J306" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L306" s="2" t="s">
         <v>8</v>
@@ -15827,7 +15836,7 @@
         <v>150</v>
       </c>
       <c r="J307" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L307" s="2" t="s">
         <v>8</v>
@@ -15865,7 +15874,7 @@
         <v>150</v>
       </c>
       <c r="J308" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L308" s="2" t="s">
         <v>8</v>
@@ -15903,7 +15912,7 @@
         <v>150</v>
       </c>
       <c r="J309" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L309" s="2" t="s">
         <v>8</v>
@@ -15941,7 +15950,7 @@
         <v>150</v>
       </c>
       <c r="J310" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L310" s="2" t="s">
         <v>8</v>
@@ -15979,7 +15988,7 @@
         <v>150</v>
       </c>
       <c r="J311" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L311" s="2" t="s">
         <v>8</v>
@@ -16017,7 +16026,7 @@
         <v>150</v>
       </c>
       <c r="J312" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L312" s="2" t="s">
         <v>8</v>
@@ -16055,7 +16064,7 @@
         <v>150</v>
       </c>
       <c r="J313" t="s">
-        <v>763</v>
+        <v>1212</v>
       </c>
       <c r="L313" s="2" t="s">
         <v>8</v>
@@ -16093,7 +16102,7 @@
         <v>150</v>
       </c>
       <c r="J314" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L314" s="2" t="s">
         <v>8</v>
@@ -16131,7 +16140,7 @@
         <v>150</v>
       </c>
       <c r="J315" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L315" s="2" t="s">
         <v>8</v>
@@ -16169,7 +16178,7 @@
         <v>150</v>
       </c>
       <c r="J316" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L316" s="2" t="s">
         <v>8</v>
@@ -16207,7 +16216,7 @@
         <v>150</v>
       </c>
       <c r="J317" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L317" s="2" t="s">
         <v>8</v>
@@ -16245,7 +16254,7 @@
         <v>150</v>
       </c>
       <c r="J318" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L318" s="2" t="s">
         <v>8</v>
@@ -16283,7 +16292,7 @@
         <v>150</v>
       </c>
       <c r="J319" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L319" s="2" t="s">
         <v>8</v>
@@ -16321,7 +16330,7 @@
         <v>150</v>
       </c>
       <c r="J320" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L320" s="2" t="s">
         <v>8</v>
@@ -16359,7 +16368,7 @@
         <v>150</v>
       </c>
       <c r="J321" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L321" s="2" t="s">
         <v>8</v>
@@ -16397,7 +16406,7 @@
         <v>150</v>
       </c>
       <c r="J322" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L322" s="2" t="s">
         <v>8</v>
@@ -16435,7 +16444,7 @@
         <v>150</v>
       </c>
       <c r="J323" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L323" s="2" t="s">
         <v>8</v>
@@ -16473,7 +16482,7 @@
         <v>150</v>
       </c>
       <c r="J324" t="s">
-        <v>762</v>
+        <v>1211</v>
       </c>
       <c r="L324" s="2" t="s">
         <v>8</v>
@@ -16511,7 +16520,7 @@
         <v>150</v>
       </c>
       <c r="J325" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L325" s="2" t="s">
         <v>8</v>
@@ -16549,7 +16558,7 @@
         <v>150</v>
       </c>
       <c r="J326" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L326" s="2" t="s">
         <v>8</v>
@@ -16587,7 +16596,7 @@
         <v>150</v>
       </c>
       <c r="J327" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L327" s="2" t="s">
         <v>8</v>
@@ -16625,7 +16634,7 @@
         <v>150</v>
       </c>
       <c r="J328" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L328" s="2" t="s">
         <v>8</v>
@@ -16663,7 +16672,7 @@
         <v>150</v>
       </c>
       <c r="J329" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L329" s="2" t="s">
         <v>8</v>
@@ -16701,7 +16710,7 @@
         <v>150</v>
       </c>
       <c r="J330" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L330" s="2" t="s">
         <v>8</v>
@@ -16739,7 +16748,7 @@
         <v>150</v>
       </c>
       <c r="J331" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L331" s="2" t="s">
         <v>8</v>
@@ -16777,7 +16786,7 @@
         <v>150</v>
       </c>
       <c r="J332" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L332" s="2" t="s">
         <v>8</v>
@@ -16815,7 +16824,7 @@
         <v>150</v>
       </c>
       <c r="J333" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L333" s="2" t="s">
         <v>8</v>
@@ -16853,7 +16862,7 @@
         <v>150</v>
       </c>
       <c r="J334" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L334" s="2" t="s">
         <v>8</v>
@@ -16891,7 +16900,7 @@
         <v>150</v>
       </c>
       <c r="J335" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L335" s="2" t="s">
         <v>8</v>
@@ -16929,7 +16938,7 @@
         <v>150</v>
       </c>
       <c r="J336" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L336" s="2" t="s">
         <v>8</v>
@@ -16967,7 +16976,7 @@
         <v>150</v>
       </c>
       <c r="J337" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L337" s="2" t="s">
         <v>8</v>
@@ -17005,7 +17014,7 @@
         <v>150</v>
       </c>
       <c r="J338" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L338" s="2" t="s">
         <v>8</v>
@@ -17043,7 +17052,7 @@
         <v>150</v>
       </c>
       <c r="J339" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L339" s="2" t="s">
         <v>8</v>
@@ -17081,7 +17090,7 @@
         <v>150</v>
       </c>
       <c r="J340" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L340" s="2" t="s">
         <v>8</v>
@@ -17119,7 +17128,7 @@
         <v>150</v>
       </c>
       <c r="J341" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L341" s="2" t="s">
         <v>8</v>
@@ -17157,7 +17166,7 @@
         <v>150</v>
       </c>
       <c r="J342" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L342" s="2" t="s">
         <v>8</v>
@@ -17195,7 +17204,7 @@
         <v>150</v>
       </c>
       <c r="J343" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L343" s="2" t="s">
         <v>8</v>
@@ -17233,7 +17242,7 @@
         <v>150</v>
       </c>
       <c r="J344" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L344" s="2" t="s">
         <v>8</v>
@@ -17271,7 +17280,7 @@
         <v>150</v>
       </c>
       <c r="J345" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L345" s="2" t="s">
         <v>8</v>
@@ -17309,7 +17318,7 @@
         <v>150</v>
       </c>
       <c r="J346" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L346" s="2" t="s">
         <v>8</v>
@@ -17347,7 +17356,7 @@
         <v>150</v>
       </c>
       <c r="J347" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L347" s="2" t="s">
         <v>8</v>
@@ -17385,7 +17394,7 @@
         <v>150</v>
       </c>
       <c r="J348" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L348" s="2" t="s">
         <v>8</v>
@@ -17423,7 +17432,7 @@
         <v>150</v>
       </c>
       <c r="J349" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L349" s="2" t="s">
         <v>8</v>
@@ -17461,7 +17470,7 @@
         <v>150</v>
       </c>
       <c r="J350" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L350" s="2" t="s">
         <v>8</v>
@@ -17499,7 +17508,7 @@
         <v>150</v>
       </c>
       <c r="J351" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L351" s="2" t="s">
         <v>8</v>
@@ -17537,7 +17546,7 @@
         <v>150</v>
       </c>
       <c r="J352" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L352" s="2" t="s">
         <v>8</v>
@@ -17575,7 +17584,7 @@
         <v>150</v>
       </c>
       <c r="J353" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L353" s="2" t="s">
         <v>8</v>
@@ -17613,7 +17622,7 @@
         <v>150</v>
       </c>
       <c r="J354" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L354" s="2" t="s">
         <v>8</v>
@@ -17651,7 +17660,7 @@
         <v>150</v>
       </c>
       <c r="J355" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L355" s="2" t="s">
         <v>8</v>
@@ -17689,7 +17698,7 @@
         <v>150</v>
       </c>
       <c r="J356" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L356" s="2" t="s">
         <v>8</v>
@@ -17727,7 +17736,7 @@
         <v>150</v>
       </c>
       <c r="J357" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L357" s="2" t="s">
         <v>8</v>
@@ -17765,7 +17774,7 @@
         <v>150</v>
       </c>
       <c r="J358" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L358" s="2" t="s">
         <v>8</v>
@@ -17803,7 +17812,7 @@
         <v>150</v>
       </c>
       <c r="J359" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L359" s="2" t="s">
         <v>8</v>
@@ -17841,7 +17850,7 @@
         <v>150</v>
       </c>
       <c r="J360" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L360" s="2" t="s">
         <v>8</v>
@@ -17879,7 +17888,7 @@
         <v>150</v>
       </c>
       <c r="J361" t="s">
-        <v>763</v>
+        <v>1211</v>
       </c>
       <c r="L361" s="2" t="s">
         <v>8</v>
@@ -17917,7 +17926,7 @@
         <v>150</v>
       </c>
       <c r="J362" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L362" s="2" t="s">
         <v>8</v>
@@ -17955,7 +17964,7 @@
         <v>150</v>
       </c>
       <c r="J363" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L363" s="2" t="s">
         <v>8</v>
@@ -17993,7 +18002,7 @@
         <v>150</v>
       </c>
       <c r="J364" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L364" s="2" t="s">
         <v>8</v>
@@ -18031,7 +18040,7 @@
         <v>150</v>
       </c>
       <c r="J365" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L365" s="2" t="s">
         <v>8</v>
@@ -18069,7 +18078,7 @@
         <v>150</v>
       </c>
       <c r="J366" t="s">
-        <v>763</v>
+        <v>1210</v>
       </c>
       <c r="L366" s="2" t="s">
         <v>8</v>
@@ -18107,7 +18116,7 @@
         <v>150</v>
       </c>
       <c r="J367" t="s">
-        <v>762</v>
+        <v>1210</v>
       </c>
       <c r="L367" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
corregir excel de events
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\racing-cayma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C05A21C-744C-4EBB-A230-0D9304B74434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913B9169-32B8-4E46-9CC2-28114C9A7A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="1212">
   <si>
     <t>XY</t>
   </si>
@@ -3656,9 +3656,6 @@
   </si>
   <si>
     <t>Ampuero</t>
-  </si>
-  <si>
-    <t>desconocido</t>
   </si>
 </sst>
 </file>
@@ -4056,8 +4053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77939FC4-FC73-4262-977F-310955BE7B1D}">
   <dimension ref="A1:N367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C121" workbookViewId="0">
-      <selection activeCell="J136" sqref="J136:J367"/>
+    <sheetView tabSelected="1" topLeftCell="C299" workbookViewId="0">
+      <selection activeCell="K316" sqref="K316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16064,7 +16061,7 @@
         <v>150</v>
       </c>
       <c r="J313" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="L313" s="2" t="s">
         <v>8</v>

</xml_diff>